<commit_message>
04/12 The sensitivity for S12_d3, S14_d3 and S14_d4_1511 is estimated, now I am finishing the Electrical Characterisation
</commit_message>
<xml_diff>
--- a/Mikhail Bandurist Transistors/Batch2_Electrical_Characterisation/MoS2_samples.xlsx
+++ b/Mikhail Bandurist Transistors/Batch2_Electrical_Characterisation/MoS2_samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Master Thesis\Mikhail Bandurist Transistors\Batch2_Electrical_Characterisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4987E512-5921-49F2-B7A3-35A05DE9DA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48B7D87-A574-4C0F-8FD1-A34CF37A3E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9E8B9CF-8318-4199-AA93-CF4BA01BF75A}"/>
   </bookViews>
@@ -45,9 +45,6 @@
     <t>ON/OFF</t>
   </si>
   <si>
-    <t>Sensitivity</t>
-  </si>
-  <si>
     <t>Measurements</t>
   </si>
   <si>
@@ -267,12 +264,6 @@
     <t>No data</t>
   </si>
   <si>
-    <t>W (channel)</t>
-  </si>
-  <si>
-    <t>L (channel)</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -364,6 +355,15 @@
   </si>
   <si>
     <t>2.67±0.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W_channel (um) </t>
+  </si>
+  <si>
+    <t>L_channel (um)</t>
+  </si>
+  <si>
+    <t>Sensitivity/Volume (C/(Gy*m^3))</t>
   </si>
 </sst>
 </file>
@@ -633,7 +633,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -725,15 +725,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1074,8 +1071,8 @@
   <dimension ref="A1:S35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35:I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1091,9 +1088,9 @@
     <col min="12" max="12" width="13" customWidth="1"/>
     <col min="13" max="13" width="28.109375" customWidth="1"/>
     <col min="14" max="14" width="19.6640625" customWidth="1"/>
-    <col min="15" max="15" width="27.5546875" style="51" customWidth="1"/>
+    <col min="15" max="15" width="27.5546875" style="48" customWidth="1"/>
     <col min="16" max="16" width="23.77734375" customWidth="1"/>
-    <col min="17" max="17" width="17.6640625" customWidth="1"/>
+    <col min="17" max="17" width="28.109375" customWidth="1"/>
     <col min="18" max="18" width="20.5546875" customWidth="1"/>
     <col min="19" max="19" width="18.88671875" customWidth="1"/>
   </cols>
@@ -1109,52 +1106,52 @@
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J1" s="35" t="s">
         <v>5</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="O1" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="P1" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="P1" s="9" t="s">
-        <v>79</v>
-      </c>
       <c r="Q1" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="R1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="S1" s="10" t="s">
         <v>7</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -1181,17 +1178,17 @@
         <v>1.24E-2</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J2" s="1">
         <f>6.38*1000000</f>
         <v>6380000</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L2" s="1">
         <v>-10.15</v>
@@ -1203,7 +1200,7 @@
         <f>40*(1/100000000)</f>
         <v>3.9999999999999998E-7</v>
       </c>
-      <c r="O2" s="49">
+      <c r="O2" s="46">
         <f>(2*E2*M2^2)/(D2*G2)*1000000</f>
         <v>0.20382360703812319</v>
       </c>
@@ -1213,10 +1210,10 @@
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S2" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -1239,17 +1236,17 @@
         <v>1.24E-2</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J3" s="1">
         <f>2.62*10000000</f>
         <v>26200000</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L3" s="1">
         <v>6.9</v>
@@ -1261,7 +1258,7 @@
         <f>7*(1/100000000)</f>
         <v>7.0000000000000005E-8</v>
       </c>
-      <c r="O3" s="49">
+      <c r="O3" s="46">
         <f>(2*E3*M3^2)/(D3*G3)*1000000</f>
         <v>1.6843934232480536E-2</v>
       </c>
@@ -1271,10 +1268,10 @@
       </c>
       <c r="Q3" s="1"/>
       <c r="R3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -1297,17 +1294,17 @@
         <v>1.24E-2</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4" s="1">
         <f>2.87*10000000</f>
         <v>28700000</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L4" s="1">
         <v>-32.1</v>
@@ -1319,7 +1316,7 @@
         <f>31.3*(1/100000000)</f>
         <v>3.1300000000000001E-7</v>
       </c>
-      <c r="O4" s="49">
+      <c r="O4" s="46">
         <f>(2*E4*M4^2)/(D4*G4)*1000000</f>
         <v>4.9033532410225197E-3</v>
       </c>
@@ -1329,10 +1326,10 @@
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S4" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
@@ -1355,17 +1352,17 @@
         <v>1.24E-2</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J5" s="1">
         <f>1.8*100000000</f>
         <v>180000000</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L5" s="1">
         <v>4.55</v>
@@ -1377,7 +1374,7 @@
         <f>2.32*(1/100000000)</f>
         <v>2.3199999999999999E-8</v>
       </c>
-      <c r="O5" s="49">
+      <c r="O5" s="46">
         <f>(2*E5*M5^2)/(D5*G5)*1000000</f>
         <v>1.0909033632697945E-2</v>
       </c>
@@ -1387,10 +1384,10 @@
       </c>
       <c r="Q5" s="1"/>
       <c r="R5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -1413,38 +1410,38 @@
         <v>1.24E-2</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K6" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M6" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N6" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="O6" s="50" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="O6" s="47" t="s">
+        <v>43</v>
       </c>
       <c r="P6" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q6" s="25"/>
       <c r="R6" s="26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="S6" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -1469,16 +1466,16 @@
         <v>1.24E-2</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J7" s="36">
         <v>425000000</v>
       </c>
       <c r="K7" s="30" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L7" s="30">
         <v>-43</v>
@@ -1491,7 +1488,7 @@
         <f>1.59/1000000</f>
         <v>1.59E-6</v>
       </c>
-      <c r="O7" s="53">
+      <c r="O7" s="50">
         <f>(2*E7*M7^2)/(D7*G7)*1000000</f>
         <v>0.47815996204933603</v>
       </c>
@@ -1501,10 +1498,10 @@
       </c>
       <c r="Q7" s="31"/>
       <c r="R7" s="32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S7" s="33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
@@ -1529,37 +1526,37 @@
         <v>1.24E-2</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J8" s="34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O8" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="P8" s="41" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="O8" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="P8" t="s">
+        <v>43</v>
       </c>
       <c r="R8" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="S8" s="18" t="s">
         <v>28</v>
-      </c>
-      <c r="S8" s="18" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -1582,16 +1579,16 @@
         <v>1.24E-2</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J9">
         <v>259259.25925925927</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L9" s="1">
         <v>-4.62</v>
@@ -1604,19 +1601,19 @@
         <f>7/100000000</f>
         <v>7.0000000000000005E-8</v>
       </c>
-      <c r="O9" s="51">
-        <f t="shared" ref="O8:O35" si="1">(2*E9*M9^2)/(D9*G9)*1000000</f>
+      <c r="O9" s="48">
+        <f t="shared" ref="O9:O35" si="1">(2*E9*M9^2)/(D9*G9)*1000000</f>
         <v>1.112665534804754E-2</v>
       </c>
-      <c r="P9" s="41">
-        <f t="shared" ref="P8:P11" si="2">(4*N9*E9*M9)/(G9*D9)*1000000</f>
+      <c r="P9">
+        <f t="shared" ref="P9" si="2">(4*N9*E9*M9)/(G9*D9)*1000000</f>
         <v>6.0848896434634996E-5</v>
       </c>
       <c r="R9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S9" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="S9" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -1639,37 +1636,37 @@
         <v>1.24E-2</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O10" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="O10" s="46" t="s">
+        <v>43</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S10" s="18" t="s">
         <v>32</v>
-      </c>
-      <c r="S10" s="18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -1679,10 +1676,10 @@
         <v>4</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F11" s="25">
         <v>278</v>
@@ -1692,38 +1689,38 @@
         <v>1.24E-2</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I11" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K11" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M11" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N11" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="O11" s="50" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="O11" s="47" t="s">
+        <v>43</v>
       </c>
       <c r="P11" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q11" s="37"/>
       <c r="R11" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S11" s="38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -1748,16 +1745,16 @@
         <v>1.24E-2</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J12" s="1">
         <v>120443448.27586205</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L12">
         <v>-15.6</v>
@@ -1770,7 +1767,7 @@
         <f>8.8/10000000</f>
         <v>8.8000000000000004E-7</v>
       </c>
-      <c r="O12" s="51">
+      <c r="O12" s="48">
         <f t="shared" si="1"/>
         <v>0.96002272547728773</v>
       </c>
@@ -1779,10 +1776,10 @@
         <v>6.7102462146148775E-3</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S12" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -1805,37 +1802,37 @@
         <v>1.24E-2</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O13" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="O13" s="46" t="s">
+        <v>43</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R13" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="S13" s="15" t="s">
         <v>38</v>
-      </c>
-      <c r="S13" s="15" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -1858,16 +1855,16 @@
         <v>1.24E-2</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I14" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J14" s="39">
         <v>1680000000</v>
       </c>
       <c r="K14" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L14" s="37">
         <v>-6.3</v>
@@ -1880,20 +1877,20 @@
         <f>2.8/10000000</f>
         <v>2.7999999999999997E-7</v>
       </c>
-      <c r="O14" s="52">
+      <c r="O14" s="49">
         <f t="shared" si="1"/>
         <v>0.26281658986175122</v>
       </c>
       <c r="P14" s="37">
-        <f t="shared" ref="P13:P35" si="3">(4*N14*E14*M14)/(G14*D14)*1000000</f>
+        <f t="shared" ref="P14:P35" si="3">(4*N14*E14*M14)/(G14*D14)*1000000</f>
         <v>1.3780645161290323E-3</v>
       </c>
       <c r="Q14" s="37"/>
       <c r="R14" s="26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S14" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -1918,16 +1915,16 @@
         <v>1.24E-2</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J15" s="1">
         <v>222333333.33333334</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="L15">
         <v>-3.2</v>
@@ -1940,7 +1937,7 @@
         <f>2.2/10000000</f>
         <v>2.2000000000000001E-7</v>
       </c>
-      <c r="O15" s="51">
+      <c r="O15" s="48">
         <f t="shared" si="1"/>
         <v>4.829953225806452E-2</v>
       </c>
@@ -1949,10 +1946,10 @@
         <v>5.3530967741935486E-4</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S15" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
@@ -1975,16 +1972,16 @@
         <v>1.24E-2</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J16" s="1">
         <v>467032.96703296708</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L16">
         <v>-9</v>
@@ -1997,7 +1994,7 @@
         <f>4/100000000</f>
         <v>4.0000000000000001E-8</v>
       </c>
-      <c r="O16" s="51">
+      <c r="O16" s="48">
         <f t="shared" si="1"/>
         <v>9.1849228611500695E-3</v>
       </c>
@@ -2006,10 +2003,10 @@
         <v>3.8877980364656386E-5</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2032,38 +2029,38 @@
         <v>1.24E-2</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K17" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L17" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M17" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N17" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="O17" s="50" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="O17" s="47" t="s">
+        <v>43</v>
       </c>
       <c r="P17" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q17" s="37"/>
       <c r="R17" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S17" s="38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -2088,16 +2085,16 @@
         <v>1.24E-2</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I18" s="30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J18" s="30">
         <v>249589.49096880128</v>
       </c>
       <c r="K18" s="30" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="L18" s="31">
         <v>10.8</v>
@@ -2110,7 +2107,7 @@
         <f>2.6/10000000</f>
         <v>2.6E-7</v>
       </c>
-      <c r="O18" s="53">
+      <c r="O18" s="50">
         <f t="shared" si="1"/>
         <v>0.24427380015735645</v>
       </c>
@@ -2120,10 +2117,10 @@
       </c>
       <c r="Q18" s="31"/>
       <c r="R18" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="S18" s="44" t="s">
-        <v>37</v>
+        <v>45</v>
+      </c>
+      <c r="S18" s="43" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
@@ -2148,42 +2145,42 @@
         <v>1.24E-2</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J19" s="42">
+        <v>46</v>
+      </c>
+      <c r="J19" s="41">
         <v>2756410.2564102565</v>
       </c>
-      <c r="K19" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="L19" s="43">
+      <c r="K19" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="L19" s="42">
         <v>-31.7</v>
       </c>
-      <c r="M19" s="43">
+      <c r="M19" s="42">
         <f>3.9/100000</f>
         <v>3.8999999999999999E-5</v>
       </c>
-      <c r="N19" s="43">
+      <c r="N19" s="42">
         <f>6.3/10000000</f>
         <v>6.3E-7</v>
       </c>
-      <c r="O19" s="54">
+      <c r="O19" s="51">
         <f t="shared" si="1"/>
         <v>2.8581271531475102E-2</v>
       </c>
-      <c r="P19" s="43">
+      <c r="P19" s="42">
         <f t="shared" si="3"/>
         <v>9.2339492640150327E-4</v>
       </c>
-      <c r="Q19" s="43"/>
+      <c r="Q19" s="42"/>
       <c r="R19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="S19" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="S19" s="15" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -2206,16 +2203,16 @@
         <v>1.24E-2</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J20" s="39">
         <v>16300000</v>
       </c>
       <c r="K20" s="25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="L20" s="37">
         <v>-14.1</v>
@@ -2228,7 +2225,7 @@
         <f>1.18/1000000</f>
         <v>1.1799999999999999E-6</v>
       </c>
-      <c r="O20" s="52">
+      <c r="O20" s="49">
         <f t="shared" si="1"/>
         <v>0.78402903225806486</v>
       </c>
@@ -2238,10 +2235,10 @@
       </c>
       <c r="Q20" s="37"/>
       <c r="R20" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="S20" s="45" t="s">
-        <v>37</v>
+        <v>48</v>
+      </c>
+      <c r="S20" s="44" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
@@ -2266,37 +2263,37 @@
         <v>1.24E-2</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="O21" s="55" t="s">
-        <v>92</v>
+        <v>89</v>
+      </c>
+      <c r="O21" s="52" t="s">
+        <v>89</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S21" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -2319,16 +2316,16 @@
         <v>1.24E-2</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J22" s="1">
         <v>58500000</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="L22">
         <v>22.3</v>
@@ -2341,7 +2338,7 @@
         <f>4.51/10000000</f>
         <v>4.51E-7</v>
       </c>
-      <c r="O22" s="51">
+      <c r="O22" s="48">
         <f t="shared" si="1"/>
         <v>1.9664457831325297E-2</v>
       </c>
@@ -2350,10 +2347,10 @@
         <v>6.3574698795180714E-4</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S22" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -2376,16 +2373,16 @@
         <v>1.24E-2</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J23" s="1">
         <v>2706074.6268656715</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L23">
         <v>-28.4</v>
@@ -2398,7 +2395,7 @@
         <f>5/10000000</f>
         <v>4.9999999999999998E-7</v>
       </c>
-      <c r="O23" s="51">
+      <c r="O23" s="48">
         <f t="shared" si="1"/>
         <v>0.71316836853098164</v>
       </c>
@@ -2407,10 +2404,10 @@
         <v>3.6951728939429102E-3</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S23" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
@@ -2433,40 +2430,40 @@
         <v>1.24E-2</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O24" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="O24" s="46" t="s">
+        <v>43</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S24" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -2489,16 +2486,16 @@
         <v>1.24E-2</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J25" s="25">
         <v>27213.930348258709</v>
       </c>
       <c r="K25" s="25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="L25" s="37">
         <v>-45</v>
@@ -2511,7 +2508,7 @@
         <f>6/10000000</f>
         <v>5.9999999999999997E-7</v>
       </c>
-      <c r="O25" s="52">
+      <c r="O25" s="49">
         <f t="shared" si="1"/>
         <v>0.32874559721011332</v>
       </c>
@@ -2521,10 +2518,10 @@
       </c>
       <c r="Q25" s="37"/>
       <c r="R25" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="S25" s="45" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="S25" s="44" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -2549,18 +2546,18 @@
         <v>1.24E-2</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J26" s="1">
         <v>78500000</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L26" s="46">
+        <v>93</v>
+      </c>
+      <c r="L26">
         <v>20</v>
       </c>
       <c r="M26">
@@ -2571,7 +2568,7 @@
         <f>4/10000000</f>
         <v>3.9999999999999998E-7</v>
       </c>
-      <c r="O26" s="51">
+      <c r="O26" s="48">
         <f t="shared" si="1"/>
         <v>3.0874204446381864E-2</v>
       </c>
@@ -2580,10 +2577,10 @@
         <v>8.4298169136878809E-4</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S26" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -2606,18 +2603,18 @@
         <v>1.24E-2</v>
       </c>
       <c r="H27" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I27" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J27" s="25">
         <v>72156862.74509804</v>
       </c>
       <c r="K27" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="L27" s="47">
+        <v>94</v>
+      </c>
+      <c r="L27" s="37">
         <v>-25</v>
       </c>
       <c r="M27" s="37">
@@ -2628,7 +2625,7 @@
         <f>2/10000000</f>
         <v>1.9999999999999999E-7</v>
       </c>
-      <c r="O27" s="52">
+      <c r="O27" s="49">
         <f t="shared" si="1"/>
         <v>0.34808702175543893</v>
       </c>
@@ -2638,10 +2635,10 @@
       </c>
       <c r="Q27" s="37"/>
       <c r="R27" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="S27" s="45" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="S27" s="44" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -2663,40 +2660,40 @@
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O28" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
+      </c>
+      <c r="O28" s="46" t="s">
+        <v>43</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S28" s="18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -2719,18 +2716,18 @@
         <v>1.24E-2</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J29" s="1">
         <v>158054.71124620063</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L29" s="46">
+        <v>95</v>
+      </c>
+      <c r="L29">
         <v>5</v>
       </c>
       <c r="M29">
@@ -2741,7 +2738,7 @@
         <f>4.3/10000000</f>
         <v>4.2999999999999996E-7</v>
       </c>
-      <c r="O29" s="51">
+      <c r="O29" s="48">
         <f t="shared" si="1"/>
         <v>0.12306818181818184</v>
       </c>
@@ -2750,10 +2747,10 @@
         <v>1.8568181818181821E-3</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S29" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -2776,18 +2773,18 @@
         <v>1.24E-2</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J30" s="1">
         <v>94932.781799379532</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L30" s="46">
+        <v>96</v>
+      </c>
+      <c r="L30">
         <v>-8</v>
       </c>
       <c r="M30">
@@ -2798,7 +2795,7 @@
         <f>1.5/10000000</f>
         <v>1.4999999999999999E-7</v>
       </c>
-      <c r="O30" s="51">
+      <c r="O30" s="48">
         <f t="shared" si="1"/>
         <v>6.7695161290322589E-2</v>
       </c>
@@ -2806,11 +2803,12 @@
         <f t="shared" si="3"/>
         <v>4.3209677419354839E-4</v>
       </c>
+      <c r="Q30" s="1"/>
       <c r="R30" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S30" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -2833,18 +2831,18 @@
         <v>1.24E-2</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I31" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J31" s="25">
         <v>235000000</v>
       </c>
       <c r="K31" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="L31" s="47">
+        <v>97</v>
+      </c>
+      <c r="L31" s="37">
         <v>-10.199999999999999</v>
       </c>
       <c r="M31" s="37">
@@ -2855,7 +2853,7 @@
         <f>1.5/10000000</f>
         <v>1.4999999999999999E-7</v>
       </c>
-      <c r="O31" s="52">
+      <c r="O31" s="49">
         <f t="shared" si="1"/>
         <v>3.310810810810811E-2</v>
       </c>
@@ -2865,10 +2863,10 @@
       </c>
       <c r="Q31" s="37"/>
       <c r="R31" s="26" t="s">
-        <v>63</v>
-      </c>
-      <c r="S31" s="56" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="S31" s="53" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -2893,18 +2891,18 @@
         <v>1.24E-2</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J32" s="1">
         <v>2055000000.0000002</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L32" s="46">
+        <v>98</v>
+      </c>
+      <c r="L32">
         <v>-10</v>
       </c>
       <c r="M32">
@@ -2915,7 +2913,7 @@
         <f>4.4/10000000</f>
         <v>4.4000000000000002E-7</v>
       </c>
-      <c r="O32" s="51">
+      <c r="O32" s="48">
         <f t="shared" si="1"/>
         <v>0.35293239447921682</v>
       </c>
@@ -2924,10 +2922,10 @@
         <v>2.7705665222275719E-3</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S32" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -2950,18 +2948,18 @@
         <v>1.24E-2</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J33" s="1">
         <v>259259259.25925922</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="L33" s="46">
+        <v>99</v>
+      </c>
+      <c r="L33">
         <v>-42</v>
       </c>
       <c r="M33">
@@ -2972,7 +2970,7 @@
         <f>9/10000000</f>
         <v>8.9999999999999996E-7</v>
       </c>
-      <c r="O33" s="51">
+      <c r="O33" s="48">
         <f t="shared" si="1"/>
         <v>0.28800000000000009</v>
       </c>
@@ -2981,10 +2979,10 @@
         <v>5.5741935483870977E-3</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S33" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
@@ -3007,18 +3005,18 @@
         <v>1.24E-2</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J34" s="1">
         <v>2420000000</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="L34" s="46">
+        <v>100</v>
+      </c>
+      <c r="L34">
         <v>-13.2</v>
       </c>
       <c r="M34">
@@ -3029,7 +3027,7 @@
         <f>8/100000000</f>
         <v>8.0000000000000002E-8</v>
       </c>
-      <c r="O34" s="51">
+      <c r="O34" s="48">
         <f t="shared" si="1"/>
         <v>0.12696300259899099</v>
       </c>
@@ -3038,10 +3036,10 @@
         <v>3.0319523008714272E-4</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S34" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:19" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -3064,16 +3062,16 @@
         <v>1.24E-2</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J35" s="6">
         <v>295333333.33333337</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L35" s="21">
         <v>-55.3</v>
@@ -3086,7 +3084,7 @@
         <f>1.1/1000000</f>
         <v>1.1000000000000001E-6</v>
       </c>
-      <c r="O35" s="51">
+      <c r="O35" s="48">
         <f t="shared" si="1"/>
         <v>0.27395405192761607</v>
       </c>
@@ -3096,10 +3094,10 @@
       </c>
       <c r="Q35" s="21"/>
       <c r="R35" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="S35" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
06/12/2023 Electrical Characterisation Report Plots are reformatted aand arranged in slides
</commit_message>
<xml_diff>
--- a/Mikhail Bandurist Transistors/Batch2_Electrical_Characterisation/MoS2_samples.xlsx
+++ b/Mikhail Bandurist Transistors/Batch2_Electrical_Characterisation/MoS2_samples.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Master Thesis\Mikhail Bandurist Transistors\Batch2_Electrical_Characterisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48B7D87-A574-4C0F-8FD1-A34CF37A3E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8F4871-7712-451A-B61B-4F1330ACA890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9E8B9CF-8318-4199-AA93-CF4BA01BF75A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="156">
   <si>
     <t>batch</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Encapsulation</t>
-  </si>
-  <si>
-    <t>ON/OFF</t>
   </si>
   <si>
     <t>Measurements</t>
@@ -312,9 +309,6 @@
     <t>9.57±0.12</t>
   </si>
   <si>
-    <t>4.03±0.03</t>
-  </si>
-  <si>
     <t>4.19±0.05</t>
   </si>
   <si>
@@ -364,6 +358,165 @@
   </si>
   <si>
     <t>Sensitivity/Volume (C/(Gy*m^3))</t>
+  </si>
+  <si>
+    <t>Vth error (V)</t>
+  </si>
+  <si>
+    <t>I1/2 intercept (A1/2)</t>
+  </si>
+  <si>
+    <t>I1/2 Inter err</t>
+  </si>
+  <si>
+    <t>Not reliable</t>
+  </si>
+  <si>
+    <t>-8.75±0.11</t>
+  </si>
+  <si>
+    <t>6.87±0.13</t>
+  </si>
+  <si>
+    <t>-32.1±-.7</t>
+  </si>
+  <si>
+    <t>4.6±0.3</t>
+  </si>
+  <si>
+    <t>-43.0±0.6</t>
+  </si>
+  <si>
+    <t>-4.62±0.08</t>
+  </si>
+  <si>
+    <t>-15.61±0.07</t>
+  </si>
+  <si>
+    <t>-6.30±0.10</t>
+  </si>
+  <si>
+    <t>-3.2±0.2</t>
+  </si>
+  <si>
+    <t>-9.23±0.08</t>
+  </si>
+  <si>
+    <t>10.76±0.16</t>
+  </si>
+  <si>
+    <t>-14.14±0.09</t>
+  </si>
+  <si>
+    <t>22.3±0.8</t>
+  </si>
+  <si>
+    <t>-28.37±0.08</t>
+  </si>
+  <si>
+    <t>-45.0±0.4</t>
+  </si>
+  <si>
+    <t>20.2±0.7</t>
+  </si>
+  <si>
+    <t>-25.02±0.9</t>
+  </si>
+  <si>
+    <t>5.1±0.3</t>
+  </si>
+  <si>
+    <t>-8.11±0.09</t>
+  </si>
+  <si>
+    <t>-10.20±0.10</t>
+  </si>
+  <si>
+    <t>-10.31±0.10</t>
+  </si>
+  <si>
+    <t>-42.1±0.5</t>
+  </si>
+  <si>
+    <t>-13.22±0.05</t>
+  </si>
+  <si>
+    <t>-55.3±0.7</t>
+  </si>
+  <si>
+    <t>0.2156±0.0013</t>
+  </si>
+  <si>
+    <t>0.01684±0.00010</t>
+  </si>
+  <si>
+    <t>0.0049±0.0002</t>
+  </si>
+  <si>
+    <t>0.01091±0.00002</t>
+  </si>
+  <si>
+    <t>0.478±0.012</t>
+  </si>
+  <si>
+    <t>0.01113±0.00006</t>
+  </si>
+  <si>
+    <t>0.96±0.007</t>
+  </si>
+  <si>
+    <t>0.26280±0.0014</t>
+  </si>
+  <si>
+    <t>0.0483±0.0005</t>
+  </si>
+  <si>
+    <t>0.00919±0.00004</t>
+  </si>
+  <si>
+    <t>0.2443±0.0016</t>
+  </si>
+  <si>
+    <t>0.784±0.006</t>
+  </si>
+  <si>
+    <t>0.0197±0.0006</t>
+  </si>
+  <si>
+    <t>0.713±0.004</t>
+  </si>
+  <si>
+    <t>0.329±0.005</t>
+  </si>
+  <si>
+    <t>0.0309±0.0008</t>
+  </si>
+  <si>
+    <t>0.3481±0.0017</t>
+  </si>
+  <si>
+    <t>0.1231±0.0019</t>
+  </si>
+  <si>
+    <t>0.0677±0.0004</t>
+  </si>
+  <si>
+    <t>0.0331±0.0003</t>
+  </si>
+  <si>
+    <t>0.353±0.003</t>
+  </si>
+  <si>
+    <t>0.288±0.006</t>
+  </si>
+  <si>
+    <t>0.1267±0.0003</t>
+  </si>
+  <si>
+    <t>0.274±0.007</t>
+  </si>
+  <si>
+    <t>ON/OFF (#/1000000)</t>
   </si>
 </sst>
 </file>
@@ -633,7 +786,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -710,18 +863,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -748,6 +894,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1068,11 +1229,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879A3825-C697-4DF2-9C86-0190DF0EBED1}">
-  <dimension ref="A1:S35"/>
+  <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35:I35"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1084,18 +1245,21 @@
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" customWidth="1"/>
     <col min="9" max="9" width="23.6640625" customWidth="1"/>
-    <col min="10" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="28.109375" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" customWidth="1"/>
-    <col min="15" max="15" width="27.5546875" style="48" customWidth="1"/>
-    <col min="16" max="16" width="23.77734375" customWidth="1"/>
-    <col min="17" max="17" width="28.109375" customWidth="1"/>
-    <col min="18" max="18" width="20.5546875" customWidth="1"/>
-    <col min="19" max="19" width="18.88671875" customWidth="1"/>
+    <col min="10" max="10" width="13" style="52" customWidth="1"/>
+    <col min="11" max="11" width="13" style="1" customWidth="1"/>
+    <col min="12" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="21.44140625" customWidth="1"/>
+    <col min="15" max="15" width="23.6640625" customWidth="1"/>
+    <col min="16" max="16" width="28.109375" customWidth="1"/>
+    <col min="17" max="17" width="19.6640625" customWidth="1"/>
+    <col min="18" max="18" width="27.5546875" style="45" customWidth="1"/>
+    <col min="19" max="19" width="23.77734375" customWidth="1"/>
+    <col min="20" max="20" width="28.109375" customWidth="1"/>
+    <col min="21" max="21" width="20.5546875" customWidth="1"/>
+    <col min="22" max="22" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1106,55 +1270,64 @@
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="51" t="s">
+        <v>155</v>
+      </c>
+      <c r="K1" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="U1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="O1" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="R1" s="9" t="s">
+      <c r="V1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="10" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>2</v>
       </c>
@@ -1178,45 +1351,54 @@
         <v>1.24E-2</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1">
-        <f>6.38*1000000</f>
-        <v>6380000</v>
+        <v>7</v>
+      </c>
+      <c r="J2" s="52">
+        <v>0.224</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L2" s="1">
-        <v>-10.15</v>
+        <v>67</v>
+      </c>
+      <c r="L2" s="53" t="s">
+        <v>107</v>
       </c>
       <c r="M2" s="1">
-        <v>9.8099999999999999E-5</v>
+        <v>-0.11206500568259056</v>
       </c>
       <c r="N2" s="1">
-        <f>40*(1/100000000)</f>
-        <v>3.9999999999999998E-7</v>
-      </c>
-      <c r="O2" s="46">
-        <f>(2*E2*M2^2)/(D2*G2)*1000000</f>
-        <v>0.20382360703812319</v>
+        <f>8.83/10000</f>
+        <v>8.83E-4</v>
+      </c>
+      <c r="O2" s="1">
+        <f>0.11/10000</f>
+        <v>1.1E-5</v>
       </c>
       <c r="P2" s="1">
-        <f>(4*N2*E2*M2)/(G2*D2)*1000000</f>
-        <v>1.6621700879765396E-3</v>
-      </c>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>16</v>
+        <f>1.009/10000</f>
+        <v>1.0089999999999999E-4</v>
+      </c>
+      <c r="Q2" s="1">
+        <f>0.003/10000</f>
+        <v>2.9999999999999999E-7</v>
+      </c>
+      <c r="R2" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="T2" s="1"/>
+      <c r="U2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="12"/>
       <c r="C3" s="1">
@@ -1236,45 +1418,53 @@
         <v>1.24E-2</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1">
-        <f>2.62*10000000</f>
-        <v>26200000</v>
+        <v>9</v>
+      </c>
+      <c r="J3" s="52">
+        <v>4.1799999999999997E-2</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L3" s="1">
-        <v>6.9</v>
+        <v>76</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="M3" s="1">
+        <v>0.13269227663193661</v>
+      </c>
+      <c r="N3" s="1">
+        <f>-1.58/10000</f>
+        <v>-1.5800000000000002E-4</v>
+      </c>
+      <c r="O3" s="1">
+        <f>0.03/10000</f>
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="P3" s="1">
         <v>2.2950000000000002E-5</v>
       </c>
-      <c r="N3" s="1">
+      <c r="Q3" s="1">
         <f>7*(1/100000000)</f>
         <v>7.0000000000000005E-8</v>
       </c>
-      <c r="O3" s="46">
-        <f>(2*E3*M3^2)/(D3*G3)*1000000</f>
-        <v>1.6843934232480536E-2</v>
-      </c>
-      <c r="P3" s="1">
-        <f>(4*N3*E3*M3)/(G3*D3)*1000000</f>
-        <v>1.0275166852057843E-4</v>
-      </c>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>17</v>
+      <c r="R3" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="T3" s="1"/>
+      <c r="U3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="1">
@@ -1294,45 +1484,52 @@
         <v>1.24E-2</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="1">
-        <f>2.87*10000000</f>
-        <v>28700000</v>
+        <v>10</v>
+      </c>
+      <c r="J4" s="52">
+        <v>3.23</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="L4" s="1">
-        <v>-32.1</v>
+        <v>77</v>
+      </c>
+      <c r="L4" s="53" t="s">
+        <v>109</v>
       </c>
       <c r="M4" s="1">
+        <v>-0.65059131789867142</v>
+      </c>
+      <c r="N4" s="1">
+        <v>5.0400000000000002E-3</v>
+      </c>
+      <c r="O4" s="1">
+        <f>3/1000000</f>
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="P4" s="1">
         <v>1.5449999999999999E-5</v>
       </c>
-      <c r="N4" s="1">
+      <c r="Q4" s="1">
         <f>31.3*(1/100000000)</f>
         <v>3.1300000000000001E-7</v>
       </c>
-      <c r="O4" s="46">
-        <f>(2*E4*M4^2)/(D4*G4)*1000000</f>
-        <v>4.9033532410225197E-3</v>
-      </c>
-      <c r="P4" s="1">
-        <f>(4*N4*E4*M4)/(G4*D4)*1000000</f>
-        <v>1.9867308277541086E-4</v>
-      </c>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="S4" s="14" t="s">
-        <v>18</v>
+      <c r="R4" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="S4" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="T4" s="1"/>
+      <c r="U4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V4" s="14" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="1">
@@ -1352,45 +1549,53 @@
         <v>1.24E-2</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="1">
-        <f>1.8*100000000</f>
-        <v>180000000</v>
+        <v>11</v>
+      </c>
+      <c r="J5" s="52">
+        <v>5.3099999999999996E-3</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="L5" s="1">
-        <v>4.55</v>
+        <v>78</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="M5" s="1">
+        <v>0.28051782942436615</v>
+      </c>
+      <c r="N5" s="1">
+        <f>-1.46/10000</f>
+        <v>-1.46E-4</v>
+      </c>
+      <c r="O5" s="1">
+        <f>0.09/10000</f>
+        <v>9.0000000000000002E-6</v>
+      </c>
+      <c r="P5" s="1">
         <v>2.2750000000000001E-5</v>
       </c>
-      <c r="N5" s="1">
+      <c r="Q5" s="1">
         <f>2.32*(1/100000000)</f>
         <v>2.3199999999999999E-8</v>
       </c>
-      <c r="O5" s="46">
-        <f>(2*E5*M5^2)/(D5*G5)*1000000</f>
-        <v>1.0909033632697945E-2</v>
-      </c>
-      <c r="P5" s="1">
-        <f>(4*N5*E5*M5)/(G5*D5)*1000000</f>
-        <v>2.2249633431085043E-5</v>
-      </c>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>19</v>
+      <c r="R5" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="S5" s="1">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="T5" s="1"/>
+      <c r="U5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="23"/>
       <c r="B6" s="24"/>
       <c r="C6" s="25">
@@ -1410,41 +1615,50 @@
         <v>1.24E-2</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="25" t="s">
-        <v>43</v>
+        <v>12</v>
+      </c>
+      <c r="J6" s="52" t="s">
+        <v>42</v>
       </c>
       <c r="K6" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="M6" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="N6" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="O6" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="O6" s="25" t="s">
+        <v>42</v>
       </c>
       <c r="P6" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="S6" s="27" t="s">
-        <v>20</v>
+        <v>42</v>
+      </c>
+      <c r="Q6" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="R6" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="T6" s="25"/>
+      <c r="U6" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="V6" s="27" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="28"/>
       <c r="B7" s="29">
         <v>4</v>
@@ -1466,45 +1680,52 @@
         <v>1.24E-2</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="36">
-        <v>425000000</v>
+        <v>20</v>
+      </c>
+      <c r="J7" s="52">
+        <v>11.3</v>
       </c>
       <c r="K7" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="L7" s="30">
-        <v>-43</v>
-      </c>
-      <c r="M7" s="31">
+        <v>79</v>
+      </c>
+      <c r="L7" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="M7" s="1">
+        <v>-0.56494137176462667</v>
+      </c>
+      <c r="N7" s="30">
+        <v>5.6299999999999996E-3</v>
+      </c>
+      <c r="O7" s="30">
+        <v>3.0000000000000001E-5</v>
+      </c>
+      <c r="P7" s="31">
         <f>1.324/10000</f>
         <v>1.3240000000000002E-4</v>
       </c>
-      <c r="N7" s="31">
+      <c r="Q7" s="31">
         <f>1.59/1000000</f>
         <v>1.59E-6</v>
       </c>
-      <c r="O7" s="50">
-        <f>(2*E7*M7^2)/(D7*G7)*1000000</f>
-        <v>0.47815996204933603</v>
-      </c>
-      <c r="P7" s="31">
-        <f>(4*N7*E7*M7)/(G7*D7)*1000000</f>
-        <v>1.1484506641366228E-2</v>
-      </c>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="S7" s="33" t="s">
-        <v>30</v>
+      <c r="R7" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="S7" s="31">
+        <v>1.2E-2</v>
+      </c>
+      <c r="T7" s="31"/>
+      <c r="U7" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="V7" s="33" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="12">
         <v>5</v>
@@ -1526,40 +1747,49 @@
         <v>1.24E-2</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="34" t="s">
-        <v>43</v>
+        <v>22</v>
+      </c>
+      <c r="J8" s="52" t="s">
+        <v>42</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O8" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="P8" t="s">
-        <v>43</v>
-      </c>
-      <c r="R8" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R8" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="S8" t="s">
+        <v>42</v>
+      </c>
+      <c r="U8" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="V8" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="S8" s="18" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="9" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="12"/>
       <c r="C9" s="1">
@@ -1579,44 +1809,53 @@
         <v>1.24E-2</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9">
-        <v>259259.25925925927</v>
+        <v>23</v>
+      </c>
+      <c r="J9" s="52">
+        <v>3.5200000000000002E-2</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="L9" s="1">
-        <v>-4.62</v>
-      </c>
-      <c r="M9">
+        <v>80</v>
+      </c>
+      <c r="L9" s="53" t="s">
+        <v>112</v>
+      </c>
+      <c r="M9" s="1">
+        <v>-7.9317553219329928E-2</v>
+      </c>
+      <c r="N9" s="1">
+        <f>1.18/10000</f>
+        <v>1.18E-4</v>
+      </c>
+      <c r="O9" s="1">
+        <f>0.02/10000</f>
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="P9">
         <f>2.56/100000</f>
         <v>2.5599999999999999E-5</v>
       </c>
-      <c r="N9">
+      <c r="Q9">
         <f>7/100000000</f>
         <v>7.0000000000000005E-8</v>
       </c>
-      <c r="O9" s="48">
-        <f t="shared" ref="O9:O35" si="1">(2*E9*M9^2)/(D9*G9)*1000000</f>
-        <v>1.112665534804754E-2</v>
-      </c>
-      <c r="P9">
-        <f t="shared" ref="P9" si="2">(4*N9*E9*M9)/(G9*D9)*1000000</f>
-        <v>6.0848896434634996E-5</v>
-      </c>
-      <c r="R9" s="2" t="s">
+      <c r="R9" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="S9">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="V9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="S9" s="4" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="10" spans="1:19" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="12"/>
       <c r="C10" s="1">
@@ -1636,50 +1875,59 @@
         <v>1.24E-2</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
+      </c>
+      <c r="J10" s="52" t="s">
+        <v>42</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O10" s="46" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R10" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V10" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="S10" s="18" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="11" spans="1:19" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="24"/>
       <c r="C11" s="25">
         <v>4</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F11" s="25">
         <v>278</v>
@@ -1689,41 +1937,50 @@
         <v>1.24E-2</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I11" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="25" t="s">
-        <v>43</v>
+        <v>25</v>
+      </c>
+      <c r="J11" s="52" t="s">
+        <v>42</v>
       </c>
       <c r="K11" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="N11" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="O11" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="O11" s="25" t="s">
+        <v>42</v>
       </c>
       <c r="P11" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="S11" s="38" t="s">
-        <v>28</v>
+        <v>42</v>
+      </c>
+      <c r="Q11" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="R11" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="S11" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="T11" s="35"/>
+      <c r="U11" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="V11" s="36" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="12">
         <v>6</v>
@@ -1745,44 +2002,51 @@
         <v>1.24E-2</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="1">
-        <v>120443448.27586205</v>
+        <v>32</v>
+      </c>
+      <c r="J12" s="52">
+        <v>14.2</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L12">
-        <v>-15.6</v>
-      </c>
-      <c r="M12">
+        <v>81</v>
+      </c>
+      <c r="L12" s="55" t="s">
+        <v>113</v>
+      </c>
+      <c r="M12" s="1">
+        <v>-6.5181751795262033E-2</v>
+      </c>
+      <c r="N12">
+        <v>3.9300000000000003E-3</v>
+      </c>
+      <c r="O12">
+        <v>9.0000000000000002E-6</v>
+      </c>
+      <c r="P12">
         <f>2.518/10000</f>
         <v>2.5179999999999999E-4</v>
       </c>
-      <c r="N12">
+      <c r="Q12">
         <f>8.8/10000000</f>
         <v>8.8000000000000004E-7</v>
       </c>
-      <c r="O12" s="48">
-        <f t="shared" si="1"/>
-        <v>0.96002272547728773</v>
-      </c>
-      <c r="P12">
-        <f>(4*N12*E12*M12)/(G12*D12)*1000000</f>
-        <v>6.7102462146148775E-3</v>
-      </c>
-      <c r="R12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S12" s="14" t="s">
-        <v>36</v>
+      <c r="R12" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="S12">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V12" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="12"/>
       <c r="C13" s="1">
@@ -1802,40 +2066,49 @@
         <v>1.24E-2</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="J13" s="52" t="s">
+        <v>42</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O13" s="46" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R13" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="R13" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U13" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="V13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="S13" s="15" t="s">
-        <v>38</v>
-      </c>
     </row>
-    <row r="14" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="24"/>
       <c r="C14" s="25">
@@ -1855,45 +2128,54 @@
         <v>1.24E-2</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I14" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="J14" s="39">
-        <v>1680000000</v>
+        <v>34</v>
+      </c>
+      <c r="J14" s="52">
+        <v>20.7</v>
       </c>
       <c r="K14" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="L14" s="37">
-        <v>-6.3</v>
-      </c>
-      <c r="M14" s="37">
+        <v>82</v>
+      </c>
+      <c r="L14" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="M14" s="1">
+        <v>-0.10443932252188505</v>
+      </c>
+      <c r="N14" s="35">
+        <f>6.72/10000</f>
+        <v>6.7199999999999996E-4</v>
+      </c>
+      <c r="O14" s="35">
+        <f>0.11/10000</f>
+        <v>1.1E-5</v>
+      </c>
+      <c r="P14" s="35">
         <f>1.068/10000</f>
         <v>1.0680000000000001E-4</v>
       </c>
-      <c r="N14" s="37">
+      <c r="Q14" s="35">
         <f>2.8/10000000</f>
         <v>2.7999999999999997E-7</v>
       </c>
-      <c r="O14" s="49">
-        <f t="shared" si="1"/>
-        <v>0.26281658986175122</v>
-      </c>
-      <c r="P14" s="37">
-        <f t="shared" ref="P14:P35" si="3">(4*N14*E14*M14)/(G14*D14)*1000000</f>
-        <v>1.3780645161290323E-3</v>
-      </c>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="S14" s="40" t="s">
-        <v>39</v>
+      <c r="R14" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="S14" s="35">
+        <v>1.4E-3</v>
+      </c>
+      <c r="T14" s="35"/>
+      <c r="U14" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="V14" s="37" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="12">
         <v>7</v>
@@ -1915,44 +2197,53 @@
         <v>1.24E-2</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J15" s="1">
-        <v>222333333.33333334</v>
+        <v>39</v>
+      </c>
+      <c r="J15" s="52">
+        <v>3.18</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L15">
-        <v>-3.2</v>
-      </c>
-      <c r="M15">
+        <v>83</v>
+      </c>
+      <c r="L15" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="M15" s="1">
+        <v>-0.20235330603789878</v>
+      </c>
+      <c r="N15">
+        <f>1.27/10000</f>
+        <v>1.27E-4</v>
+      </c>
+      <c r="O15">
+        <f>0.08/10000</f>
+        <v>7.9999999999999996E-6</v>
+      </c>
+      <c r="P15">
         <f>3.97/100000</f>
         <v>3.9700000000000003E-5</v>
       </c>
-      <c r="N15">
+      <c r="Q15">
         <f>2.2/10000000</f>
         <v>2.2000000000000001E-7</v>
       </c>
-      <c r="O15" s="48">
-        <f t="shared" si="1"/>
-        <v>4.829953225806452E-2</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="3"/>
-        <v>5.3530967741935486E-4</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="S15" s="14" t="s">
-        <v>36</v>
+      <c r="R15" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="S15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V15" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="12"/>
       <c r="C16" s="1">
@@ -1972,44 +2263,53 @@
         <v>1.24E-2</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J16" s="1">
-        <v>467032.96703296708</v>
+        <v>40</v>
+      </c>
+      <c r="J16" s="52">
+        <v>3.98E-3</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L16">
-        <v>-9</v>
-      </c>
-      <c r="M16">
+        <v>84</v>
+      </c>
+      <c r="L16" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="M16" s="1">
+        <v>-7.6652967337003886E-2</v>
+      </c>
+      <c r="N16">
+        <f>1.697/10000</f>
+        <v>1.697E-4</v>
+      </c>
+      <c r="O16">
+        <f>0.014/10000</f>
+        <v>1.3999999999999999E-6</v>
+      </c>
+      <c r="P16">
         <f>1.89/100000</f>
         <v>1.8899999999999999E-5</v>
       </c>
-      <c r="N16">
+      <c r="Q16">
         <f>4/100000000</f>
         <v>4.0000000000000001E-8</v>
       </c>
-      <c r="O16" s="48">
-        <f t="shared" si="1"/>
-        <v>9.1849228611500695E-3</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="3"/>
-        <v>3.8877980364656386E-5</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S16" s="4" t="s">
-        <v>30</v>
+      <c r="R16" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="S16">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V16" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="24"/>
       <c r="C17" s="25">
@@ -2029,41 +2329,50 @@
         <v>1.24E-2</v>
       </c>
       <c r="H17" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I17" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="J17" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="J17" s="52" t="s">
+        <v>42</v>
       </c>
       <c r="K17" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L17" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="M17" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="N17" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="O17" s="47" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="P17" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q17" s="37"/>
-      <c r="R17" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="S17" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="Q17" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="R17" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="S17" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="T17" s="35"/>
+      <c r="U17" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="V17" s="36" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="29">
         <v>8</v>
@@ -2085,45 +2394,54 @@
         <v>1.24E-2</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I18" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="J18" s="30">
-        <v>249589.49096880128</v>
+        <v>43</v>
+      </c>
+      <c r="J18" s="52">
+        <v>1.7399999999999999E-2</v>
       </c>
       <c r="K18" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="L18" s="31">
-        <v>10.8</v>
-      </c>
-      <c r="M18" s="31">
+        <v>85</v>
+      </c>
+      <c r="L18" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0.15623087106417624</v>
+      </c>
+      <c r="N18" s="31">
+        <f>-8.52/10000</f>
+        <v>-8.52E-4</v>
+      </c>
+      <c r="O18" s="31">
+        <f>0.12/10000</f>
+        <v>1.2E-5</v>
+      </c>
+      <c r="P18" s="31">
         <f>7.88/100000</f>
         <v>7.8800000000000004E-5</v>
       </c>
-      <c r="N18" s="31">
+      <c r="Q18" s="31">
         <f>2.6/10000000</f>
         <v>2.6E-7</v>
       </c>
-      <c r="O18" s="50">
-        <f t="shared" si="1"/>
-        <v>0.24427380015735645</v>
-      </c>
-      <c r="P18" s="31">
-        <f t="shared" si="3"/>
-        <v>1.611959087332809E-3</v>
-      </c>
-      <c r="Q18" s="31"/>
-      <c r="R18" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="S18" s="43" t="s">
-        <v>36</v>
+      <c r="R18" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="S18" s="31">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="T18" s="31"/>
+      <c r="U18" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="V18" s="40" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
       <c r="B19" s="12">
         <v>9</v>
@@ -2145,45 +2463,48 @@
         <v>1.24E-2</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J19" s="41">
-        <v>2756410.2564102565</v>
-      </c>
-      <c r="K19" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="L19" s="42">
-        <v>-31.7</v>
-      </c>
-      <c r="M19" s="42">
+        <v>45</v>
+      </c>
+      <c r="J19" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="K19" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="L19" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39"/>
+      <c r="P19" s="39">
         <f>3.9/100000</f>
         <v>3.8999999999999999E-5</v>
       </c>
-      <c r="N19" s="42">
+      <c r="Q19" s="39">
         <f>6.3/10000000</f>
         <v>6.3E-7</v>
       </c>
-      <c r="O19" s="51">
-        <f t="shared" si="1"/>
+      <c r="R19" s="48">
         <v>2.8581271531475102E-2</v>
       </c>
-      <c r="P19" s="42">
-        <f t="shared" si="3"/>
-        <v>9.2339492640150327E-4</v>
-      </c>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="2" t="s">
+      <c r="S19" s="39">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="T19" s="39"/>
+      <c r="U19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V19" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="S19" s="15" t="s">
-        <v>49</v>
-      </c>
     </row>
-    <row r="20" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="B20" s="24"/>
       <c r="C20" s="25">
@@ -2203,45 +2524,52 @@
         <v>1.24E-2</v>
       </c>
       <c r="H20" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I20" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="J20" s="39">
-        <v>16300000</v>
+        <v>46</v>
+      </c>
+      <c r="J20" s="52">
+        <v>0.81599999999999995</v>
       </c>
       <c r="K20" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="L20" s="37">
-        <v>-14.1</v>
-      </c>
-      <c r="M20" s="37">
+        <v>86</v>
+      </c>
+      <c r="L20" s="56" t="s">
+        <v>118</v>
+      </c>
+      <c r="M20" s="1">
+        <v>-8.7960442907750208E-2</v>
+      </c>
+      <c r="N20" s="35">
+        <v>4.1700000000000001E-3</v>
+      </c>
+      <c r="O20" s="35">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="P20" s="35">
         <f>2.958/10000</f>
         <v>2.9580000000000003E-4</v>
       </c>
-      <c r="N20" s="37">
+      <c r="Q20" s="35">
         <f>1.18/1000000</f>
         <v>1.1799999999999999E-6</v>
       </c>
-      <c r="O20" s="49">
-        <f t="shared" si="1"/>
-        <v>0.78402903225806486</v>
-      </c>
-      <c r="P20" s="37">
-        <f t="shared" si="3"/>
-        <v>6.2552688172043021E-3</v>
-      </c>
-      <c r="Q20" s="37"/>
-      <c r="R20" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="S20" s="44" t="s">
-        <v>36</v>
+      <c r="R20" s="46" t="s">
+        <v>142</v>
+      </c>
+      <c r="S20" s="35">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="T20" s="35"/>
+      <c r="U20" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="V20" s="41" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="12">
         <v>10</v>
@@ -2263,40 +2591,49 @@
         <v>1.24E-2</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>89</v>
+        <v>49</v>
+      </c>
+      <c r="J21" s="52" t="s">
+        <v>87</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="O21" s="52" t="s">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="R21" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S21" s="18" t="s">
-        <v>43</v>
+        <v>87</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="R21" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="V21" s="18" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="12"/>
       <c r="C22" s="1">
@@ -2316,44 +2653,53 @@
         <v>1.24E-2</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="J22" s="1">
-        <v>58500000</v>
+        <v>50</v>
+      </c>
+      <c r="J22" s="52">
+        <v>0.5</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L22">
-        <v>22.3</v>
-      </c>
-      <c r="M22">
+        <v>88</v>
+      </c>
+      <c r="L22" t="s">
+        <v>119</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0.8046209275346744</v>
+      </c>
+      <c r="N22">
+        <f>-6.2/100000</f>
+        <v>-6.2000000000000003E-5</v>
+      </c>
+      <c r="O22">
+        <f>0.2/100000</f>
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="P22">
         <f>2.79/100000</f>
         <v>2.7900000000000001E-5</v>
       </c>
-      <c r="N22">
+      <c r="Q22">
         <f>4.51/10000000</f>
         <v>4.51E-7</v>
       </c>
-      <c r="O22" s="48">
-        <f t="shared" si="1"/>
-        <v>1.9664457831325297E-2</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="3"/>
-        <v>6.3574698795180714E-4</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="S22" s="14" t="s">
-        <v>36</v>
+      <c r="R22" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="S22">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="U22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="V22" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="16"/>
       <c r="B23" s="12"/>
       <c r="C23" s="1">
@@ -2373,44 +2719,51 @@
         <v>1.24E-2</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J23" s="1">
-        <v>2706074.6268656715</v>
+        <v>51</v>
+      </c>
+      <c r="J23" s="52">
+        <v>0.21099999999999999</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="L23">
-        <v>-28.4</v>
-      </c>
-      <c r="M23">
+        <v>89</v>
+      </c>
+      <c r="L23" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="M23" s="1">
+        <v>-7.9898250219780351E-2</v>
+      </c>
+      <c r="N23">
+        <v>5.47E-3</v>
+      </c>
+      <c r="O23">
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="P23">
         <f>1.93/10000</f>
         <v>1.93E-4</v>
       </c>
-      <c r="N23">
+      <c r="Q23">
         <f>5/10000000</f>
         <v>4.9999999999999998E-7</v>
       </c>
-      <c r="O23" s="48">
-        <f t="shared" si="1"/>
-        <v>0.71316836853098164</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="3"/>
-        <v>3.6951728939429102E-3</v>
-      </c>
-      <c r="R23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="S23" s="14" t="s">
-        <v>36</v>
+      <c r="R23" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="S23">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="U23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="V23" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="12"/>
       <c r="C24" s="1">
@@ -2430,43 +2783,52 @@
         <v>1.24E-2</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
+      </c>
+      <c r="J24" s="52" t="s">
+        <v>42</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O24" s="46" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R24" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="S24" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="R24" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V24" s="18" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="24"/>
       <c r="C25" s="25">
@@ -2486,45 +2848,53 @@
         <v>1.24E-2</v>
       </c>
       <c r="H25" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="J25" s="25">
-        <v>27213.930348258709</v>
+        <v>53</v>
+      </c>
+      <c r="J25" s="52">
+        <v>9.8200000000000006E-3</v>
       </c>
       <c r="K25" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="L25" s="37">
-        <v>-45</v>
-      </c>
-      <c r="M25" s="37">
+        <v>90</v>
+      </c>
+      <c r="L25" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="M25" s="1">
+        <v>-0.35693767442191798</v>
+      </c>
+      <c r="N25" s="35">
+        <f>0.00372</f>
+        <v>3.7200000000000002E-3</v>
+      </c>
+      <c r="O25" s="35">
+        <v>1.2E-5</v>
+      </c>
+      <c r="P25" s="35">
         <f>8.28/100000</f>
         <v>8.2799999999999993E-5</v>
       </c>
-      <c r="N25" s="37">
+      <c r="Q25" s="35">
         <f>6/10000000</f>
         <v>5.9999999999999997E-7</v>
       </c>
-      <c r="O25" s="49">
-        <f t="shared" si="1"/>
-        <v>0.32874559721011332</v>
-      </c>
-      <c r="P25" s="37">
-        <f t="shared" si="3"/>
-        <v>4.764428945074106E-3</v>
-      </c>
-      <c r="Q25" s="37"/>
-      <c r="R25" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="S25" s="44" t="s">
-        <v>36</v>
+      <c r="R25" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="S25" s="35">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="T25" s="35"/>
+      <c r="U25" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="V25" s="41" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
       <c r="B26" s="12">
         <v>11</v>
@@ -2546,44 +2916,53 @@
         <v>1.24E-2</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J26" s="1">
-        <v>78500000</v>
+        <v>56</v>
+      </c>
+      <c r="J26" s="52">
+        <v>6.4300000000000002E-4</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="L26">
-        <v>20</v>
-      </c>
-      <c r="M26">
+        <v>91</v>
+      </c>
+      <c r="L26" t="s">
+        <v>122</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0.71611533958052664</v>
+      </c>
+      <c r="N26">
+        <f>-5.74/10000</f>
+        <v>-5.7400000000000007E-4</v>
+      </c>
+      <c r="O26">
+        <f>0.19/10000</f>
+        <v>1.9000000000000001E-5</v>
+      </c>
+      <c r="P26">
         <f>2.93/100000</f>
         <v>2.9300000000000001E-5</v>
       </c>
-      <c r="N26">
+      <c r="Q26">
         <f>4/10000000</f>
         <v>3.9999999999999998E-7</v>
       </c>
-      <c r="O26" s="48">
-        <f t="shared" si="1"/>
-        <v>3.0874204446381864E-2</v>
-      </c>
-      <c r="P26">
-        <f t="shared" si="3"/>
-        <v>8.4298169136878809E-4</v>
-      </c>
-      <c r="R26" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="S26" s="14" t="s">
-        <v>36</v>
+      <c r="R26" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="S26">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="U26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="V26" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="24"/>
       <c r="C27" s="25">
@@ -2603,45 +2982,53 @@
         <v>1.24E-2</v>
       </c>
       <c r="H27" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I27" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="J27" s="25">
-        <v>72156862.74509804</v>
+        <v>57</v>
+      </c>
+      <c r="J27" s="52">
+        <v>6.44</v>
       </c>
       <c r="K27" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="L27" s="37">
-        <v>-25</v>
-      </c>
-      <c r="M27" s="37">
+        <v>92</v>
+      </c>
+      <c r="L27" s="56" t="s">
+        <v>123</v>
+      </c>
+      <c r="M27" s="1">
+        <v>-8.0039052967910598E-2</v>
+      </c>
+      <c r="N27" s="35">
+        <v>2E-3</v>
+      </c>
+      <c r="O27" s="35">
+        <f>4/1000000</f>
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="P27" s="35">
         <f>8/100000</f>
         <v>8.0000000000000007E-5</v>
       </c>
-      <c r="N27" s="37">
+      <c r="Q27" s="35">
         <f>2/10000000</f>
         <v>1.9999999999999999E-7</v>
       </c>
-      <c r="O27" s="49">
-        <f t="shared" si="1"/>
-        <v>0.34808702175543893</v>
-      </c>
-      <c r="P27" s="37">
-        <f t="shared" si="3"/>
-        <v>1.7404351087771943E-3</v>
-      </c>
-      <c r="Q27" s="37"/>
-      <c r="R27" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="S27" s="44" t="s">
-        <v>36</v>
+      <c r="R27" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="S27" s="35">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="T27" s="35"/>
+      <c r="U27" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="V27" s="41" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="12">
         <v>12</v>
@@ -2658,45 +3045,57 @@
       <c r="F28" s="1">
         <v>278</v>
       </c>
-      <c r="G28" s="1"/>
+      <c r="G28" s="25">
+        <f t="shared" si="0"/>
+        <v>1.24E-2</v>
+      </c>
       <c r="H28" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>43</v>
+        <v>58</v>
+      </c>
+      <c r="J28" s="52" t="s">
+        <v>42</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="O28" s="46" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="R28" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="S28" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="R28" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V28" s="18" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="16"/>
       <c r="B29" s="12"/>
       <c r="C29" s="1">
@@ -2716,44 +3115,53 @@
         <v>1.24E-2</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J29" s="1">
-        <v>158054.71124620063</v>
+        <v>20</v>
+      </c>
+      <c r="J29" s="52">
+        <v>6.7599999999999993E-2</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L29">
-        <v>5</v>
-      </c>
-      <c r="M29">
+        <v>93</v>
+      </c>
+      <c r="L29" t="s">
+        <v>124</v>
+      </c>
+      <c r="M29" s="1">
+        <v>0.31913828999068994</v>
+      </c>
+      <c r="N29">
+        <f>-2.84/10000</f>
+        <v>-2.8399999999999996E-4</v>
+      </c>
+      <c r="O29">
+        <f>0.18/10000</f>
+        <v>1.8E-5</v>
+      </c>
+      <c r="P29">
         <f>5.7/100000</f>
         <v>5.7000000000000003E-5</v>
       </c>
-      <c r="N29">
+      <c r="Q29">
         <f>4.3/10000000</f>
         <v>4.2999999999999996E-7</v>
       </c>
-      <c r="O29" s="48">
-        <f t="shared" si="1"/>
-        <v>0.12306818181818184</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="3"/>
-        <v>1.8568181818181821E-3</v>
-      </c>
-      <c r="R29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="S29" s="14" t="s">
-        <v>36</v>
+      <c r="R29" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="S29">
+        <v>1.9E-3</v>
+      </c>
+      <c r="U29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="V29" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="12"/>
       <c r="C30" s="1">
@@ -2773,45 +3181,54 @@
         <v>1.24E-2</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J30" s="1">
-        <v>94932.781799379532</v>
+        <v>59</v>
+      </c>
+      <c r="J30" s="52">
+        <v>3.2599999999999999E-3</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L30">
-        <v>-8</v>
-      </c>
-      <c r="M30">
+        <v>94</v>
+      </c>
+      <c r="L30" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="M30" s="1">
+        <v>-8.9071075304571687E-2</v>
+      </c>
+      <c r="N30">
+        <f>3.75/10000</f>
+        <v>3.7500000000000001E-4</v>
+      </c>
+      <c r="O30">
+        <f>0.04/10000</f>
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="P30">
         <f>4.7/100000</f>
         <v>4.7000000000000004E-5</v>
       </c>
-      <c r="N30">
+      <c r="Q30">
         <f>1.5/10000000</f>
         <v>1.4999999999999999E-7</v>
       </c>
-      <c r="O30" s="48">
-        <f t="shared" si="1"/>
-        <v>6.7695161290322589E-2</v>
-      </c>
-      <c r="P30">
-        <f t="shared" si="3"/>
-        <v>4.3209677419354839E-4</v>
-      </c>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="S30" s="5" t="s">
-        <v>63</v>
+      <c r="R30" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="S30">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="T30" s="1"/>
+      <c r="U30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="V30" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="24"/>
       <c r="C31" s="25">
@@ -2831,45 +3248,54 @@
         <v>1.24E-2</v>
       </c>
       <c r="H31" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I31" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="J31" s="25">
-        <v>235000000</v>
+        <v>60</v>
+      </c>
+      <c r="J31" s="52">
+        <v>1.08</v>
       </c>
       <c r="K31" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="L31" s="37">
-        <v>-10.199999999999999</v>
-      </c>
-      <c r="M31" s="37">
+        <v>95</v>
+      </c>
+      <c r="L31" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="M31" s="1">
+        <v>-9.5164725912389475E-2</v>
+      </c>
+      <c r="N31" s="35">
+        <f>3.62/10000</f>
+        <v>3.6200000000000002E-4</v>
+      </c>
+      <c r="O31" s="35">
+        <f>0.03/10000</f>
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="P31" s="35">
         <f>3.5/100000</f>
         <v>3.4999999999999997E-5</v>
       </c>
-      <c r="N31" s="37">
+      <c r="Q31" s="35">
         <f>1.5/10000000</f>
         <v>1.4999999999999999E-7</v>
       </c>
-      <c r="O31" s="49">
-        <f t="shared" si="1"/>
-        <v>3.310810810810811E-2</v>
-      </c>
-      <c r="P31" s="37">
-        <f t="shared" si="3"/>
-        <v>2.8378378378378371E-4</v>
-      </c>
-      <c r="Q31" s="37"/>
-      <c r="R31" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="S31" s="53" t="s">
-        <v>64</v>
+      <c r="R31" s="46" t="s">
+        <v>150</v>
+      </c>
+      <c r="S31" s="35">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="T31" s="35"/>
+      <c r="U31" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="V31" s="50" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="12">
         <v>14</v>
@@ -2891,44 +3317,51 @@
         <v>1.24E-2</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="J32" s="1">
-        <v>2055000000.0000002</v>
+        <v>58</v>
+      </c>
+      <c r="J32" s="52">
+        <v>9.18</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L32">
-        <v>-10</v>
-      </c>
-      <c r="M32">
+        <v>96</v>
+      </c>
+      <c r="L32" s="55" t="s">
+        <v>127</v>
+      </c>
+      <c r="M32" s="1">
+        <v>-9.6809513242537004E-2</v>
+      </c>
+      <c r="N32">
+        <v>1.1299999999999999E-3</v>
+      </c>
+      <c r="O32">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="P32">
         <f>1.121/10000</f>
         <v>1.121E-4</v>
       </c>
-      <c r="N32">
+      <c r="Q32">
         <f>4.4/10000000</f>
         <v>4.4000000000000002E-7</v>
       </c>
-      <c r="O32" s="48">
-        <f t="shared" si="1"/>
-        <v>0.35293239447921682</v>
-      </c>
-      <c r="P32">
-        <f t="shared" si="3"/>
-        <v>2.7705665222275719E-3</v>
-      </c>
-      <c r="R32" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="S32" s="14" t="s">
-        <v>36</v>
+      <c r="R32" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="S32">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="U32" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V32" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="12"/>
       <c r="C33" s="1">
@@ -2948,44 +3381,51 @@
         <v>1.24E-2</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J33" s="1">
-        <v>259259259.25925922</v>
+        <v>20</v>
+      </c>
+      <c r="J33" s="52">
+        <v>15.8</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L33">
-        <v>-42</v>
-      </c>
-      <c r="M33">
+        <v>97</v>
+      </c>
+      <c r="L33" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="M33" s="1">
+        <v>-0.4592253227166484</v>
+      </c>
+      <c r="N33">
+        <v>3.9300000000000003E-3</v>
+      </c>
+      <c r="O33">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="P33">
         <f>9.3/100000</f>
         <v>9.3000000000000011E-5</v>
       </c>
-      <c r="N33">
+      <c r="Q33">
         <f>9/10000000</f>
         <v>8.9999999999999996E-7</v>
       </c>
-      <c r="O33" s="48">
-        <f t="shared" si="1"/>
-        <v>0.28800000000000009</v>
-      </c>
-      <c r="P33">
-        <f t="shared" si="3"/>
-        <v>5.5741935483870977E-3</v>
-      </c>
-      <c r="R33" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="S33" s="5" t="s">
-        <v>64</v>
+      <c r="R33" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="S33">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="U33" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V33" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="12"/>
       <c r="C34" s="1">
@@ -3005,44 +3445,53 @@
         <v>1.24E-2</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J34" s="1">
-        <v>2420000000</v>
+        <v>64</v>
+      </c>
+      <c r="J34" s="52">
+        <v>12.1</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="L34">
-        <v>-13.2</v>
-      </c>
-      <c r="M34">
+        <v>98</v>
+      </c>
+      <c r="L34" s="55" t="s">
+        <v>129</v>
+      </c>
+      <c r="M34" s="1">
+        <v>-4.7584051699129312E-2</v>
+      </c>
+      <c r="N34">
+        <f>8.82/10000</f>
+        <v>8.8200000000000008E-4</v>
+      </c>
+      <c r="O34">
+        <f>0.03/10000</f>
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="P34">
         <f>6.7/100000</f>
         <v>6.7000000000000002E-5</v>
       </c>
-      <c r="N34">
+      <c r="Q34">
         <f>8/100000000</f>
         <v>8.0000000000000002E-8</v>
       </c>
-      <c r="O34" s="48">
-        <f t="shared" si="1"/>
-        <v>0.12696300259899099</v>
-      </c>
-      <c r="P34">
-        <f t="shared" si="3"/>
-        <v>3.0319523008714272E-4</v>
-      </c>
-      <c r="R34" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="S34" s="5" t="s">
-        <v>66</v>
+      <c r="R34" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="S34">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="U34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V34" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:22" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="19"/>
       <c r="B35" s="20"/>
       <c r="C35" s="6">
@@ -3062,42 +3511,54 @@
         <v>1.24E-2</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="J35" s="6">
-        <v>295333333.33333337</v>
+        <v>60</v>
+      </c>
+      <c r="J35" s="52">
+        <v>15.7</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="L35" s="21">
-        <v>-55.3</v>
-      </c>
-      <c r="M35" s="21">
+        <v>99</v>
+      </c>
+      <c r="L35" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="M35" s="1">
+        <v>-0.68631169220488575</v>
+      </c>
+      <c r="N35" s="21">
+        <v>5.1599999999999997E-3</v>
+      </c>
+      <c r="O35" s="21">
+        <v>2.0000000000000002E-5</v>
+      </c>
+      <c r="P35" s="21">
         <f>9.33/100000</f>
         <v>9.3300000000000005E-5</v>
       </c>
-      <c r="N35" s="21">
+      <c r="Q35" s="21">
         <f>1.1/1000000</f>
         <v>1.1000000000000001E-6</v>
       </c>
-      <c r="O35" s="48">
-        <f t="shared" si="1"/>
-        <v>0.27395405192761607</v>
-      </c>
-      <c r="P35">
-        <f t="shared" si="3"/>
-        <v>6.459795436664046E-3</v>
-      </c>
-      <c r="Q35" s="21"/>
-      <c r="R35" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="S35" s="22" t="s">
-        <v>64</v>
+      <c r="R35" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="S35">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="T35" s="21"/>
+      <c r="U35" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="V35" s="22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J39" s="52">
+        <v>1000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
06/12/2023 Saved the presentation and the table, now I am writing the comments
</commit_message>
<xml_diff>
--- a/Mikhail Bandurist Transistors/Batch2_Electrical_Characterisation/MoS2_samples.xlsx
+++ b/Mikhail Bandurist Transistors/Batch2_Electrical_Characterisation/MoS2_samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Master Thesis\Mikhail Bandurist Transistors\Batch2_Electrical_Characterisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8F4871-7712-451A-B61B-4F1330ACA890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D960F2-4F3F-4255-850A-AD0B45F3CD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9E8B9CF-8318-4199-AA93-CF4BA01BF75A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="158">
   <si>
     <t>batch</t>
   </si>
@@ -517,6 +517,12 @@
   </si>
   <si>
     <t>ON/OFF (#/1000000)</t>
+  </si>
+  <si>
+    <t>Comments (more detailed)</t>
+  </si>
+  <si>
+    <t>trfSat and trfLin are fine, hysteresis is present, but small, however, the output does not show field effect, only at low VGate</t>
   </si>
 </sst>
 </file>
@@ -786,7 +792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -909,6 +915,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1229,11 +1239,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879A3825-C697-4DF2-9C86-0190DF0EBED1}">
-  <dimension ref="A1:V39"/>
+  <dimension ref="A1:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1242,7 +1252,7 @@
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="17.88671875" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" customWidth="1"/>
     <col min="9" max="9" width="23.6640625" customWidth="1"/>
     <col min="10" max="10" width="13" style="52" customWidth="1"/>
@@ -1257,9 +1267,10 @@
     <col min="20" max="20" width="28.109375" customWidth="1"/>
     <col min="21" max="21" width="20.5546875" customWidth="1"/>
     <col min="22" max="22" width="18.88671875" customWidth="1"/>
+    <col min="23" max="23" width="110.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1326,8 +1337,11 @@
       <c r="V1" s="10" t="s">
         <v>6</v>
       </c>
+      <c r="W1" s="58" t="s">
+        <v>156</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>2</v>
       </c>
@@ -1397,8 +1411,11 @@
       <c r="V2" s="13" t="s">
         <v>15</v>
       </c>
+      <c r="W2" s="59" t="s">
+        <v>157</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="12"/>
       <c r="C3" s="1">
@@ -1463,8 +1480,9 @@
       <c r="V3" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="W3" s="17"/>
     </row>
-    <row r="4" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="1">
@@ -1528,8 +1546,9 @@
       <c r="V4" s="14" t="s">
         <v>17</v>
       </c>
+      <c r="W4" s="17"/>
     </row>
-    <row r="5" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="1">
@@ -1594,8 +1613,9 @@
       <c r="V5" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="W5" s="17"/>
     </row>
-    <row r="6" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="23"/>
       <c r="B6" s="24"/>
       <c r="C6" s="25">
@@ -1657,8 +1677,9 @@
       <c r="V6" s="27" t="s">
         <v>19</v>
       </c>
+      <c r="W6" s="17"/>
     </row>
-    <row r="7" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="28"/>
       <c r="B7" s="29">
         <v>4</v>
@@ -1724,8 +1745,9 @@
       <c r="V7" s="33" t="s">
         <v>29</v>
       </c>
+      <c r="W7" s="17"/>
     </row>
-    <row r="8" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="12">
         <v>5</v>
@@ -1788,8 +1810,9 @@
       <c r="V8" s="18" t="s">
         <v>27</v>
       </c>
+      <c r="W8" s="17"/>
     </row>
-    <row r="9" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="12"/>
       <c r="C9" s="1">
@@ -1854,8 +1877,9 @@
       <c r="V9" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="W9" s="17"/>
     </row>
-    <row r="10" spans="1:22" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="12"/>
       <c r="C10" s="1">
@@ -1916,8 +1940,9 @@
       <c r="V10" s="18" t="s">
         <v>31</v>
       </c>
+      <c r="W10" s="17"/>
     </row>
-    <row r="11" spans="1:22" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="24"/>
       <c r="C11" s="25">
@@ -1979,8 +2004,9 @@
       <c r="V11" s="36" t="s">
         <v>27</v>
       </c>
+      <c r="W11" s="17"/>
     </row>
-    <row r="12" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="12">
         <v>6</v>
@@ -2045,8 +2071,9 @@
       <c r="V12" s="14" t="s">
         <v>35</v>
       </c>
+      <c r="W12" s="17"/>
     </row>
-    <row r="13" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="12"/>
       <c r="C13" s="1">
@@ -2107,8 +2134,9 @@
       <c r="V13" s="15" t="s">
         <v>37</v>
       </c>
+      <c r="W13" s="17"/>
     </row>
-    <row r="14" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="24"/>
       <c r="C14" s="25">
@@ -2174,8 +2202,9 @@
       <c r="V14" s="37" t="s">
         <v>38</v>
       </c>
+      <c r="W14" s="17"/>
     </row>
-    <row r="15" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="12">
         <v>7</v>
@@ -2242,8 +2271,9 @@
       <c r="V15" s="14" t="s">
         <v>35</v>
       </c>
+      <c r="W15" s="17"/>
     </row>
-    <row r="16" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="12"/>
       <c r="C16" s="1">
@@ -2308,8 +2338,9 @@
       <c r="V16" s="4" t="s">
         <v>29</v>
       </c>
+      <c r="W16" s="17"/>
     </row>
-    <row r="17" spans="1:22" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="24"/>
       <c r="C17" s="25">
@@ -2371,8 +2402,9 @@
       <c r="V17" s="36" t="s">
         <v>42</v>
       </c>
+      <c r="W17" s="17"/>
     </row>
-    <row r="18" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="29">
         <v>8</v>
@@ -2440,8 +2472,9 @@
       <c r="V18" s="40" t="s">
         <v>35</v>
       </c>
+      <c r="W18" s="17"/>
     </row>
-    <row r="19" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
       <c r="B19" s="12">
         <v>9</v>
@@ -2503,8 +2536,9 @@
       <c r="V19" s="15" t="s">
         <v>48</v>
       </c>
+      <c r="W19" s="17"/>
     </row>
-    <row r="20" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="B20" s="24"/>
       <c r="C20" s="25">
@@ -2568,8 +2602,9 @@
       <c r="V20" s="41" t="s">
         <v>35</v>
       </c>
+      <c r="W20" s="17"/>
     </row>
-    <row r="21" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="12">
         <v>10</v>
@@ -2632,8 +2667,9 @@
       <c r="V21" s="18" t="s">
         <v>42</v>
       </c>
+      <c r="W21" s="17"/>
     </row>
-    <row r="22" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="12"/>
       <c r="C22" s="1">
@@ -2698,8 +2734,9 @@
       <c r="V22" s="14" t="s">
         <v>35</v>
       </c>
+      <c r="W22" s="17"/>
     </row>
-    <row r="23" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="16"/>
       <c r="B23" s="12"/>
       <c r="C23" s="1">
@@ -2762,8 +2799,9 @@
       <c r="V23" s="14" t="s">
         <v>35</v>
       </c>
+      <c r="W23" s="17"/>
     </row>
-    <row r="24" spans="1:22" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="12"/>
       <c r="C24" s="1">
@@ -2827,8 +2865,9 @@
       <c r="V24" s="18" t="s">
         <v>42</v>
       </c>
+      <c r="W24" s="17"/>
     </row>
-    <row r="25" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="24"/>
       <c r="C25" s="25">
@@ -2893,8 +2932,9 @@
       <c r="V25" s="41" t="s">
         <v>35</v>
       </c>
+      <c r="W25" s="17"/>
     </row>
-    <row r="26" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
       <c r="B26" s="12">
         <v>11</v>
@@ -2961,8 +3001,9 @@
       <c r="V26" s="14" t="s">
         <v>35</v>
       </c>
+      <c r="W26" s="17"/>
     </row>
-    <row r="27" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="24"/>
       <c r="C27" s="25">
@@ -3027,8 +3068,9 @@
       <c r="V27" s="41" t="s">
         <v>35</v>
       </c>
+      <c r="W27" s="17"/>
     </row>
-    <row r="28" spans="1:22" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="12">
         <v>12</v>
@@ -3094,8 +3136,9 @@
       <c r="V28" s="18" t="s">
         <v>42</v>
       </c>
+      <c r="W28" s="17"/>
     </row>
-    <row r="29" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="16"/>
       <c r="B29" s="12"/>
       <c r="C29" s="1">
@@ -3160,8 +3203,9 @@
       <c r="V29" s="14" t="s">
         <v>35</v>
       </c>
+      <c r="W29" s="17"/>
     </row>
-    <row r="30" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="12"/>
       <c r="C30" s="1">
@@ -3227,8 +3271,9 @@
       <c r="V30" s="5" t="s">
         <v>62</v>
       </c>
+      <c r="W30" s="17"/>
     </row>
-    <row r="31" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="24"/>
       <c r="C31" s="25">
@@ -3294,8 +3339,9 @@
       <c r="V31" s="50" t="s">
         <v>63</v>
       </c>
+      <c r="W31" s="17"/>
     </row>
-    <row r="32" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="12">
         <v>14</v>
@@ -3360,8 +3406,9 @@
       <c r="V32" s="14" t="s">
         <v>35</v>
       </c>
+      <c r="W32" s="17"/>
     </row>
-    <row r="33" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="12"/>
       <c r="C33" s="1">
@@ -3424,8 +3471,9 @@
       <c r="V33" s="5" t="s">
         <v>63</v>
       </c>
+      <c r="W33" s="17"/>
     </row>
-    <row r="34" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="12"/>
       <c r="C34" s="1">
@@ -3490,8 +3538,9 @@
       <c r="V34" s="5" t="s">
         <v>65</v>
       </c>
+      <c r="W34" s="17"/>
     </row>
-    <row r="35" spans="1:22" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="19"/>
       <c r="B35" s="20"/>
       <c r="C35" s="6">
@@ -3555,8 +3604,9 @@
       <c r="V35" s="22" t="s">
         <v>63</v>
       </c>
+      <c r="W35" s="17"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="J39" s="52">
         <v>1000000</v>
       </c>

</xml_diff>

<commit_message>
Report on Electrical Characterisation is ready (only to delete the comments in the table in the beginning) and is sent to Ilaria, now I am preparing the report on the X-Ray measurements
</commit_message>
<xml_diff>
--- a/Mikhail Bandurist Transistors/Batch2_Electrical_Characterisation/MoS2_samples.xlsx
+++ b/Mikhail Bandurist Transistors/Batch2_Electrical_Characterisation/MoS2_samples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Master Thesis\Mikhail Bandurist Transistors\Batch2_Electrical_Characterisation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D960F2-4F3F-4255-850A-AD0B45F3CD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3854F9A-95E7-4EC8-ADE1-896477903CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9E8B9CF-8318-4199-AA93-CF4BA01BF75A}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{C9E8B9CF-8318-4199-AA93-CF4BA01BF75A}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="182">
   <si>
     <t>batch</t>
   </si>
@@ -270,15 +270,6 @@
     <t>mu (cm^2/(V*s))</t>
   </si>
   <si>
-    <t>I1/2 Slope (A^1/2/V)</t>
-  </si>
-  <si>
-    <t>Error I1/2 Slope</t>
-  </si>
-  <si>
-    <t>Error mu</t>
-  </si>
-  <si>
     <t>12.67±0.08</t>
   </si>
   <si>
@@ -360,15 +351,6 @@
     <t>Sensitivity/Volume (C/(Gy*m^3))</t>
   </si>
   <si>
-    <t>Vth error (V)</t>
-  </si>
-  <si>
-    <t>I1/2 intercept (A1/2)</t>
-  </si>
-  <si>
-    <t>I1/2 Inter err</t>
-  </si>
-  <si>
     <t>Not reliable</t>
   </si>
   <si>
@@ -522,14 +504,117 @@
     <t>Comments (more detailed)</t>
   </si>
   <si>
-    <t>trfSat and trfLin are fine, hysteresis is present, but small, however, the output does not show field effect, only at low VGate</t>
+    <t xml:space="preserve">No signal is observed, possibly, bad connection was present. </t>
+  </si>
+  <si>
+    <t>No signal is observed, probably, bad connection.</t>
+  </si>
+  <si>
+    <t>No signal is observed (Idrain is almost zero), probably, bad connection.</t>
+  </si>
+  <si>
+    <t>No signal is observed.</t>
+  </si>
+  <si>
+    <t>No signal was observed, probably, bad connection.</t>
+  </si>
+  <si>
+    <t>trfSat is not finished because of constant interruption from the interlock, so I used the trfSat curve that got the longest measurement range. After that the connection between the sample and the tips was completely lost.</t>
+  </si>
+  <si>
+    <t>trfSat and trfLin perform well, however, the output curves are completely linear.</t>
+  </si>
+  <si>
+    <t>trfSat and trfLin have siginificant hysteresis, the output curves show field effect only at VGate below 10V.</t>
+  </si>
+  <si>
+    <t>trfSat and trfLin perfrom well, howeverm the output curves show absolutely no field effect.</t>
+  </si>
+  <si>
+    <t>trfSat and trfLin perform well even with hysteresis, the output curves show field effect at VGate below 30V.</t>
+  </si>
+  <si>
+    <t>trfSat and trfLin have medium hysteresis, the output curves show field effect only at VGate below 10V.</t>
+  </si>
+  <si>
+    <t>trfSat and trfLin have significant hysteresis, however, the output curves show absolutely no field effect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trfSat and trfLin have significant hysteresis, however, the output curves show good field effect. </t>
+  </si>
+  <si>
+    <t>trfSat and trfLin perform well with small hysteresis, the output curves show field effect only at VGate below 30V.</t>
+  </si>
+  <si>
+    <t>trfSat and trfLin perform well with small hysteresis, the output curves show field effect only at VGate below -10V.</t>
+  </si>
+  <si>
+    <t>trfSat and trfLin perform well with small hysteresis, the output curves show field effect at VGate below 30V.</t>
+  </si>
+  <si>
+    <t>at trfSat and trfLin significant hysteresis is present, however, the output curves show good field effect.</t>
+  </si>
+  <si>
+    <t>At trfSat and trfLin hysteresis is observed, the output curves show field effect at VGate &lt;= 30V.</t>
+  </si>
+  <si>
+    <t>trfSat curve behaves well only below 0-10V (compliance?), trfLin performs well even with hysteresis, the output curves show good field effect. The measured properties are considered unreliable.</t>
+  </si>
+  <si>
+    <t>At trfSat and trfLin hysteresis is observed, the output curves show good field effect.</t>
+  </si>
+  <si>
+    <t>No signal at trfSat is observed, at VGate=10V IDrain is about 10^(-10) A. The output curves show ohmic behaviour, which implies independence of the IDrain on VGate (ignorance of the gate from the active channel).</t>
+  </si>
+  <si>
+    <t>At trfSat and trfLin significant hysteresis is observed, the output curves show absolutely no field effect.</t>
+  </si>
+  <si>
+    <t>At trfSat and trfLin significant hysteresis is observed, the output curves show good field effect.</t>
+  </si>
+  <si>
+    <t>At trfSat and trfLin hysteresis is present, output curves show good field effect.</t>
+  </si>
+  <si>
+    <t>trfSat and trfLin are fine, small hysteresis is present, the output curves show field effect at VGate &lt;= 30V.</t>
+  </si>
+  <si>
+    <t>At trfSat and trfLin significant hysteresis is observed, the output curves show no field effect.</t>
+  </si>
+  <si>
+    <t>trfSat is comparable to the one sent by Adrian, output curves show no field effect.</t>
+  </si>
+  <si>
+    <t>At trfSat and trfLin a hysteresis is significant, however the output curves show good field effect.</t>
+  </si>
+  <si>
+    <r>
+      <t>trfSat and trfLin are fine, small hysteresis is present, the output curves show field effect at VGate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;= 30V.</t>
+    </r>
+  </si>
+  <si>
+    <t>At trfSat and trfLin a hysteresis is present, the output curves show no field effect.</t>
+  </si>
+  <si>
+    <t>trfSat and trfLin are fine, hysteresis is present, but small, however, the output curves show no field effect.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -554,6 +639,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -792,7 +885,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -915,10 +1008,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1239,11 +1329,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{879A3825-C697-4DF2-9C86-0190DF0EBED1}">
-  <dimension ref="A1:W39"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W3" sqref="W3"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1255,22 +1345,17 @@
     <col min="7" max="7" width="16.33203125" customWidth="1"/>
     <col min="8" max="8" width="18.6640625" customWidth="1"/>
     <col min="9" max="9" width="23.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13" style="52" customWidth="1"/>
+    <col min="10" max="10" width="19.77734375" style="52" customWidth="1"/>
     <col min="11" max="11" width="13" style="1" customWidth="1"/>
-    <col min="12" max="13" width="13" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" customWidth="1"/>
-    <col min="15" max="15" width="23.6640625" customWidth="1"/>
-    <col min="16" max="16" width="28.109375" customWidth="1"/>
-    <col min="17" max="17" width="19.6640625" customWidth="1"/>
-    <col min="18" max="18" width="27.5546875" style="45" customWidth="1"/>
-    <col min="19" max="19" width="23.77734375" customWidth="1"/>
-    <col min="20" max="20" width="28.109375" customWidth="1"/>
-    <col min="21" max="21" width="20.5546875" customWidth="1"/>
-    <col min="22" max="22" width="18.88671875" customWidth="1"/>
-    <col min="23" max="23" width="110.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="27.5546875" style="45" customWidth="1"/>
+    <col min="14" max="14" width="28.109375" customWidth="1"/>
+    <col min="15" max="15" width="20.5546875" customWidth="1"/>
+    <col min="16" max="16" width="18.88671875" customWidth="1"/>
+    <col min="17" max="17" width="110.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1281,10 +1366,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>3</v>
@@ -1299,7 +1384,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="51" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="K1" s="34" t="s">
         <v>66</v>
@@ -1307,41 +1392,23 @@
       <c r="L1" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="M1" s="9" t="s">
-        <v>103</v>
+      <c r="M1" s="42" t="s">
+        <v>72</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="R1" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="U1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="58" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q1" s="58" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>2</v>
       </c>
@@ -1377,45 +1444,23 @@
         <v>67</v>
       </c>
       <c r="L2" s="53" t="s">
-        <v>107</v>
-      </c>
-      <c r="M2" s="1">
-        <v>-0.11206500568259056</v>
-      </c>
-      <c r="N2" s="1">
-        <f>8.83/10000</f>
-        <v>8.83E-4</v>
-      </c>
-      <c r="O2" s="1">
-        <f>0.11/10000</f>
-        <v>1.1E-5</v>
-      </c>
-      <c r="P2" s="1">
-        <f>1.009/10000</f>
-        <v>1.0089999999999999E-4</v>
-      </c>
-      <c r="Q2" s="1">
-        <f>0.003/10000</f>
-        <v>2.9999999999999999E-7</v>
-      </c>
-      <c r="R2" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="S2" s="1">
-        <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="T2" s="1"/>
-      <c r="U2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="N2" s="1"/>
+      <c r="O2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="P2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="W2" s="59" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q2" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="12"/>
       <c r="C3" s="1">
@@ -1444,45 +1489,26 @@
         <v>4.1799999999999997E-2</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0.13269227663193661</v>
-      </c>
-      <c r="N3" s="1">
-        <f>-1.58/10000</f>
-        <v>-1.5800000000000002E-4</v>
-      </c>
-      <c r="O3" s="1">
-        <f>0.03/10000</f>
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="P3" s="1">
-        <v>2.2950000000000002E-5</v>
-      </c>
-      <c r="Q3" s="1">
-        <f>7*(1/100000000)</f>
-        <v>7.0000000000000005E-8</v>
-      </c>
-      <c r="R3" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="S3" s="1">
-        <v>1E-4</v>
-      </c>
-      <c r="T3" s="1"/>
-      <c r="U3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="M3" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="W3" s="17"/>
-    </row>
-    <row r="4" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q3" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="1">
@@ -1511,44 +1537,26 @@
         <v>3.23</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="L4" s="53" t="s">
-        <v>109</v>
-      </c>
-      <c r="M4" s="1">
-        <v>-0.65059131789867142</v>
-      </c>
-      <c r="N4" s="1">
-        <v>5.0400000000000002E-3</v>
-      </c>
-      <c r="O4" s="1">
-        <f>3/1000000</f>
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="P4" s="1">
-        <v>1.5449999999999999E-5</v>
-      </c>
-      <c r="Q4" s="1">
-        <f>31.3*(1/100000000)</f>
-        <v>3.1300000000000001E-7</v>
-      </c>
-      <c r="R4" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="S4" s="1">
-        <v>2.0000000000000001E-4</v>
-      </c>
-      <c r="T4" s="1"/>
-      <c r="U4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="M4" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="N4" s="1"/>
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="14" t="s">
+      <c r="P4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="W4" s="17"/>
-    </row>
-    <row r="5" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="Q4" s="17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="1">
@@ -1577,45 +1585,26 @@
         <v>5.3099999999999996E-3</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="M5" s="1">
-        <v>0.28051782942436615</v>
-      </c>
-      <c r="N5" s="1">
-        <f>-1.46/10000</f>
-        <v>-1.46E-4</v>
-      </c>
-      <c r="O5" s="1">
-        <f>0.09/10000</f>
-        <v>9.0000000000000002E-6</v>
-      </c>
-      <c r="P5" s="1">
-        <v>2.2750000000000001E-5</v>
-      </c>
-      <c r="Q5" s="1">
-        <f>2.32*(1/100000000)</f>
-        <v>2.3199999999999999E-8</v>
-      </c>
-      <c r="R5" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="S5" s="1">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="T5" s="1"/>
-      <c r="U5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M5" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="N5" s="1"/>
+      <c r="O5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="V5" s="5" t="s">
+      <c r="P5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="W5" s="17"/>
-    </row>
-    <row r="6" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q5" s="17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="23"/>
       <c r="B6" s="24"/>
       <c r="C6" s="25">
@@ -1649,37 +1638,21 @@
       <c r="L6" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N6" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="O6" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="P6" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q6" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="R6" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="S6" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="T6" s="25"/>
-      <c r="U6" s="26" t="s">
+      <c r="M6" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="25"/>
+      <c r="O6" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="V6" s="27" t="s">
+      <c r="P6" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="W6" s="17"/>
-    </row>
-    <row r="7" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q6" s="17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="28"/>
       <c r="B7" s="29">
         <v>4</v>
@@ -1710,44 +1683,26 @@
         <v>11.3</v>
       </c>
       <c r="K7" s="30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="L7" s="54" t="s">
-        <v>111</v>
-      </c>
-      <c r="M7" s="1">
-        <v>-0.56494137176462667</v>
-      </c>
-      <c r="N7" s="30">
-        <v>5.6299999999999996E-3</v>
-      </c>
-      <c r="O7" s="30">
-        <v>3.0000000000000001E-5</v>
-      </c>
-      <c r="P7" s="31">
-        <f>1.324/10000</f>
-        <v>1.3240000000000002E-4</v>
-      </c>
-      <c r="Q7" s="31">
-        <f>1.59/1000000</f>
-        <v>1.59E-6</v>
-      </c>
-      <c r="R7" s="47" t="s">
-        <v>135</v>
-      </c>
-      <c r="S7" s="31">
-        <v>1.2E-2</v>
-      </c>
-      <c r="T7" s="31"/>
-      <c r="U7" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="M7" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="N7" s="31"/>
+      <c r="O7" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="V7" s="33" t="s">
+      <c r="P7" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="W7" s="17"/>
-    </row>
-    <row r="8" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Q7" s="17" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="12">
         <v>5</v>
@@ -1783,36 +1738,20 @@
       <c r="L8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R8" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="S8" t="s">
-        <v>42</v>
-      </c>
-      <c r="U8" s="17" t="s">
+      <c r="M8" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="V8" s="18" t="s">
+      <c r="P8" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="W8" s="17"/>
-    </row>
-    <row r="9" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q8" s="17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="12"/>
       <c r="C9" s="1">
@@ -1841,45 +1780,25 @@
         <v>3.5200000000000002E-2</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="L9" s="53" t="s">
-        <v>112</v>
-      </c>
-      <c r="M9" s="1">
-        <v>-7.9317553219329928E-2</v>
-      </c>
-      <c r="N9" s="1">
-        <f>1.18/10000</f>
-        <v>1.18E-4</v>
-      </c>
-      <c r="O9" s="1">
-        <f>0.02/10000</f>
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="P9">
-        <f>2.56/100000</f>
-        <v>2.5599999999999999E-5</v>
-      </c>
-      <c r="Q9">
-        <f>7/100000000</f>
-        <v>7.0000000000000005E-8</v>
-      </c>
-      <c r="R9" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="S9">
-        <v>6.0000000000000002E-5</v>
-      </c>
-      <c r="U9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="M9" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="O9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="V9" s="4" t="s">
+      <c r="P9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="W9" s="17"/>
-    </row>
-    <row r="10" spans="1:23" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q9" s="17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="12"/>
       <c r="C10" s="1">
@@ -1913,36 +1832,20 @@
       <c r="L10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R10" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U10" s="2" t="s">
+      <c r="M10" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="O10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="V10" s="18" t="s">
+      <c r="P10" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="W10" s="17"/>
-    </row>
-    <row r="11" spans="1:23" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q10" s="17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="24"/>
       <c r="C11" s="25">
@@ -1976,37 +1879,21 @@
       <c r="L11" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N11" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="O11" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="P11" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q11" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="R11" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="S11" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="T11" s="35"/>
-      <c r="U11" s="26" t="s">
+      <c r="M11" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="N11" s="35"/>
+      <c r="O11" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="V11" s="36" t="s">
+      <c r="P11" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="W11" s="17"/>
-    </row>
-    <row r="12" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q11" s="17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="12">
         <v>6</v>
@@ -2037,43 +1924,25 @@
         <v>14.2</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="L12" s="55" t="s">
-        <v>113</v>
-      </c>
-      <c r="M12" s="1">
-        <v>-6.5181751795262033E-2</v>
-      </c>
-      <c r="N12">
-        <v>3.9300000000000003E-3</v>
-      </c>
-      <c r="O12">
-        <v>9.0000000000000002E-6</v>
-      </c>
-      <c r="P12">
-        <f>2.518/10000</f>
-        <v>2.5179999999999999E-4</v>
-      </c>
-      <c r="Q12">
-        <f>8.8/10000000</f>
-        <v>8.8000000000000004E-7</v>
-      </c>
-      <c r="R12" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="S12">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="U12" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="M12" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="O12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V12" s="14" t="s">
+      <c r="P12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="W12" s="17"/>
-    </row>
-    <row r="13" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q12" s="17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="12"/>
       <c r="C13" s="1">
@@ -2107,36 +1976,20 @@
       <c r="L13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R13" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U13" s="17" t="s">
+      <c r="M13" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="O13" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="V13" s="15" t="s">
+      <c r="P13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="W13" s="17"/>
-    </row>
-    <row r="14" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q13" s="17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="24"/>
       <c r="C14" s="25">
@@ -2165,46 +2018,26 @@
         <v>20.7</v>
       </c>
       <c r="K14" s="25" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="L14" s="56" t="s">
-        <v>114</v>
-      </c>
-      <c r="M14" s="1">
-        <v>-0.10443932252188505</v>
-      </c>
-      <c r="N14" s="35">
-        <f>6.72/10000</f>
-        <v>6.7199999999999996E-4</v>
-      </c>
-      <c r="O14" s="35">
-        <f>0.11/10000</f>
-        <v>1.1E-5</v>
-      </c>
-      <c r="P14" s="35">
-        <f>1.068/10000</f>
-        <v>1.0680000000000001E-4</v>
-      </c>
-      <c r="Q14" s="35">
-        <f>2.8/10000000</f>
-        <v>2.7999999999999997E-7</v>
-      </c>
-      <c r="R14" s="46" t="s">
-        <v>138</v>
-      </c>
-      <c r="S14" s="35">
-        <v>1.4E-3</v>
-      </c>
-      <c r="T14" s="35"/>
-      <c r="U14" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="M14" s="46" t="s">
+        <v>132</v>
+      </c>
+      <c r="N14" s="35"/>
+      <c r="O14" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="V14" s="37" t="s">
+      <c r="P14" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="W14" s="17"/>
-    </row>
-    <row r="15" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q14" s="17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="12">
         <v>7</v>
@@ -2235,45 +2068,25 @@
         <v>3.18</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L15" s="55" t="s">
-        <v>115</v>
-      </c>
-      <c r="M15" s="1">
-        <v>-0.20235330603789878</v>
-      </c>
-      <c r="N15">
-        <f>1.27/10000</f>
-        <v>1.27E-4</v>
-      </c>
-      <c r="O15">
-        <f>0.08/10000</f>
-        <v>7.9999999999999996E-6</v>
-      </c>
-      <c r="P15">
-        <f>3.97/100000</f>
-        <v>3.9700000000000003E-5</v>
-      </c>
-      <c r="Q15">
-        <f>2.2/10000000</f>
-        <v>2.2000000000000001E-7</v>
-      </c>
-      <c r="R15" s="45" t="s">
-        <v>139</v>
-      </c>
-      <c r="S15">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="U15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="M15" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="O15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V15" s="14" t="s">
+      <c r="P15" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="W15" s="17"/>
-    </row>
-    <row r="16" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="Q15" s="17" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="12"/>
       <c r="C16" s="1">
@@ -2302,45 +2115,25 @@
         <v>3.98E-3</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L16" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="M16" s="1">
-        <v>-7.6652967337003886E-2</v>
-      </c>
-      <c r="N16">
-        <f>1.697/10000</f>
-        <v>1.697E-4</v>
-      </c>
-      <c r="O16">
-        <f>0.014/10000</f>
-        <v>1.3999999999999999E-6</v>
-      </c>
-      <c r="P16">
-        <f>1.89/100000</f>
-        <v>1.8899999999999999E-5</v>
-      </c>
-      <c r="Q16">
-        <f>4/100000000</f>
-        <v>4.0000000000000001E-8</v>
-      </c>
-      <c r="R16" s="45" t="s">
-        <v>140</v>
-      </c>
-      <c r="S16">
-        <v>4.0000000000000003E-5</v>
-      </c>
-      <c r="U16" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="M16" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="O16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="V16" s="4" t="s">
+      <c r="P16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="W16" s="17"/>
-    </row>
-    <row r="17" spans="1:23" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q16" s="17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="24"/>
       <c r="C17" s="25">
@@ -2374,37 +2167,21 @@
       <c r="L17" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P17" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q17" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="R17" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="S17" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="T17" s="35"/>
-      <c r="U17" s="26" t="s">
+      <c r="M17" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="N17" s="35"/>
+      <c r="O17" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="V17" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="W17" s="17"/>
-    </row>
-    <row r="18" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="P17" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q17" s="17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="29">
         <v>8</v>
@@ -2435,46 +2212,26 @@
         <v>1.7399999999999999E-2</v>
       </c>
       <c r="K18" s="30" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L18" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="M18" s="1">
-        <v>0.15623087106417624</v>
-      </c>
-      <c r="N18" s="31">
-        <f>-8.52/10000</f>
-        <v>-8.52E-4</v>
-      </c>
-      <c r="O18" s="31">
-        <f>0.12/10000</f>
-        <v>1.2E-5</v>
-      </c>
-      <c r="P18" s="31">
-        <f>7.88/100000</f>
-        <v>7.8800000000000004E-5</v>
-      </c>
-      <c r="Q18" s="31">
-        <f>2.6/10000000</f>
-        <v>2.6E-7</v>
-      </c>
-      <c r="R18" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="S18" s="31">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="T18" s="31"/>
-      <c r="U18" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="M18" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="N18" s="31"/>
+      <c r="O18" s="32" t="s">
         <v>44</v>
       </c>
-      <c r="V18" s="40" t="s">
+      <c r="P18" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="W18" s="17"/>
-    </row>
-    <row r="19" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="Q18" s="17" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
       <c r="B19" s="12">
         <v>9</v>
@@ -2502,43 +2259,29 @@
         <v>45</v>
       </c>
       <c r="J19" s="52" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="K19" s="38" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="L19" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
+      </c>
+      <c r="M19" s="48">
+        <v>2.8581271531475102E-2</v>
       </c>
       <c r="N19" s="39"/>
-      <c r="O19" s="39"/>
-      <c r="P19" s="39">
-        <f>3.9/100000</f>
-        <v>3.8999999999999999E-5</v>
-      </c>
-      <c r="Q19" s="39">
-        <f>6.3/10000000</f>
-        <v>6.3E-7</v>
-      </c>
-      <c r="R19" s="48">
-        <v>2.8581271531475102E-2</v>
-      </c>
-      <c r="S19" s="39">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="T19" s="39"/>
-      <c r="U19" s="2" t="s">
+      <c r="O19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="V19" s="15" t="s">
+      <c r="P19" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="W19" s="17"/>
-    </row>
-    <row r="20" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q19" s="17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="B20" s="24"/>
       <c r="C20" s="25">
@@ -2567,44 +2310,26 @@
         <v>0.81599999999999995</v>
       </c>
       <c r="K20" s="25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L20" s="56" t="s">
-        <v>118</v>
-      </c>
-      <c r="M20" s="1">
-        <v>-8.7960442907750208E-2</v>
-      </c>
-      <c r="N20" s="35">
-        <v>4.1700000000000001E-3</v>
-      </c>
-      <c r="O20" s="35">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="P20" s="35">
-        <f>2.958/10000</f>
-        <v>2.9580000000000003E-4</v>
-      </c>
-      <c r="Q20" s="35">
-        <f>1.18/1000000</f>
-        <v>1.1799999999999999E-6</v>
-      </c>
-      <c r="R20" s="46" t="s">
-        <v>142</v>
-      </c>
-      <c r="S20" s="35">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="T20" s="35"/>
-      <c r="U20" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="M20" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="N20" s="35"/>
+      <c r="O20" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="V20" s="41" t="s">
+      <c r="P20" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="W20" s="17"/>
-    </row>
-    <row r="21" spans="1:23" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="Q20" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="12">
         <v>10</v>
@@ -2632,44 +2357,28 @@
         <v>49</v>
       </c>
       <c r="J21" s="52" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
+      </c>
+      <c r="M21" s="49" t="s">
+        <v>84</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="R21" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="S21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="U21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="V21" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="W21" s="17"/>
-    </row>
-    <row r="22" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="P21" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q21" s="17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="12"/>
       <c r="C22" s="1">
@@ -2698,45 +2407,25 @@
         <v>0.5</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L22" t="s">
-        <v>119</v>
-      </c>
-      <c r="M22" s="1">
-        <v>0.8046209275346744</v>
-      </c>
-      <c r="N22">
-        <f>-6.2/100000</f>
-        <v>-6.2000000000000003E-5</v>
-      </c>
-      <c r="O22">
-        <f>0.2/100000</f>
-        <v>1.9999999999999999E-6</v>
-      </c>
-      <c r="P22">
-        <f>2.79/100000</f>
-        <v>2.7900000000000001E-5</v>
-      </c>
-      <c r="Q22">
-        <f>4.51/10000000</f>
-        <v>4.51E-7</v>
-      </c>
-      <c r="R22" s="45" t="s">
-        <v>143</v>
-      </c>
-      <c r="S22">
-        <v>5.9999999999999995E-4</v>
-      </c>
-      <c r="U22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M22" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="O22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="V22" s="14" t="s">
+      <c r="P22" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="W22" s="17"/>
-    </row>
-    <row r="23" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q22" s="17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="16"/>
       <c r="B23" s="12"/>
       <c r="C23" s="1">
@@ -2765,43 +2454,25 @@
         <v>0.21099999999999999</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="L23" s="55" t="s">
-        <v>120</v>
-      </c>
-      <c r="M23" s="1">
-        <v>-7.9898250219780351E-2</v>
-      </c>
-      <c r="N23">
-        <v>5.47E-3</v>
-      </c>
-      <c r="O23">
-        <v>6.0000000000000002E-6</v>
-      </c>
-      <c r="P23">
-        <f>1.93/10000</f>
-        <v>1.93E-4</v>
-      </c>
-      <c r="Q23">
-        <f>5/10000000</f>
-        <v>4.9999999999999998E-7</v>
-      </c>
-      <c r="R23" s="45" t="s">
-        <v>144</v>
-      </c>
-      <c r="S23">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="U23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="M23" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="O23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="V23" s="14" t="s">
+      <c r="P23" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="W23" s="17"/>
-    </row>
-    <row r="24" spans="1:23" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q23" s="17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="12"/>
       <c r="C24" s="1">
@@ -2835,39 +2506,23 @@
       <c r="L24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="M24" s="43" t="s">
         <v>42</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R24" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U24" s="2" t="s">
+      <c r="O24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="V24" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="W24" s="17"/>
-    </row>
-    <row r="25" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="P24" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q24" s="17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="24"/>
       <c r="C25" s="25">
@@ -2896,45 +2551,26 @@
         <v>9.8200000000000006E-3</v>
       </c>
       <c r="K25" s="25" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L25" s="56" t="s">
-        <v>121</v>
-      </c>
-      <c r="M25" s="1">
-        <v>-0.35693767442191798</v>
-      </c>
-      <c r="N25" s="35">
-        <f>0.00372</f>
-        <v>3.7200000000000002E-3</v>
-      </c>
-      <c r="O25" s="35">
-        <v>1.2E-5</v>
-      </c>
-      <c r="P25" s="35">
-        <f>8.28/100000</f>
-        <v>8.2799999999999993E-5</v>
-      </c>
-      <c r="Q25" s="35">
-        <f>6/10000000</f>
-        <v>5.9999999999999997E-7</v>
-      </c>
-      <c r="R25" s="46" t="s">
-        <v>145</v>
-      </c>
-      <c r="S25" s="35">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="T25" s="35"/>
-      <c r="U25" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="M25" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="N25" s="35"/>
+      <c r="O25" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="V25" s="41" t="s">
+      <c r="P25" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="W25" s="17"/>
-    </row>
-    <row r="26" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q25" s="17" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
       <c r="B26" s="12">
         <v>11</v>
@@ -2965,45 +2601,25 @@
         <v>6.4300000000000002E-4</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="L26" t="s">
-        <v>122</v>
-      </c>
-      <c r="M26" s="1">
-        <v>0.71611533958052664</v>
-      </c>
-      <c r="N26">
-        <f>-5.74/10000</f>
-        <v>-5.7400000000000007E-4</v>
-      </c>
-      <c r="O26">
-        <f>0.19/10000</f>
-        <v>1.9000000000000001E-5</v>
-      </c>
-      <c r="P26">
-        <f>2.93/100000</f>
-        <v>2.9300000000000001E-5</v>
-      </c>
-      <c r="Q26">
-        <f>4/10000000</f>
-        <v>3.9999999999999998E-7</v>
-      </c>
-      <c r="R26" s="45" t="s">
-        <v>146</v>
-      </c>
-      <c r="S26">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="U26" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="M26" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="O26" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="V26" s="14" t="s">
+      <c r="P26" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="W26" s="17"/>
-    </row>
-    <row r="27" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q26" s="17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="24"/>
       <c r="C27" s="25">
@@ -3032,45 +2648,26 @@
         <v>6.44</v>
       </c>
       <c r="K27" s="25" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L27" s="56" t="s">
-        <v>123</v>
-      </c>
-      <c r="M27" s="1">
-        <v>-8.0039052967910598E-2</v>
-      </c>
-      <c r="N27" s="35">
-        <v>2E-3</v>
-      </c>
-      <c r="O27" s="35">
-        <f>4/1000000</f>
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="P27" s="35">
-        <f>8/100000</f>
-        <v>8.0000000000000007E-5</v>
-      </c>
-      <c r="Q27" s="35">
-        <f>2/10000000</f>
-        <v>1.9999999999999999E-7</v>
-      </c>
-      <c r="R27" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="S27" s="35">
-        <v>1.6999999999999999E-3</v>
-      </c>
-      <c r="T27" s="35"/>
-      <c r="U27" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="M27" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="N27" s="35"/>
+      <c r="O27" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="V27" s="41" t="s">
+      <c r="P27" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="W27" s="17"/>
-    </row>
-    <row r="28" spans="1:23" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q27" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="12">
         <v>12</v>
@@ -3106,39 +2703,23 @@
       <c r="L28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="M28" s="43" t="s">
         <v>42</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="P28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R28" s="43" t="s">
-        <v>42</v>
-      </c>
-      <c r="S28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="U28" s="2" t="s">
+      <c r="O28" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="V28" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="W28" s="17"/>
-    </row>
-    <row r="29" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="P28" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q28" s="17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="16"/>
       <c r="B29" s="12"/>
       <c r="C29" s="1">
@@ -3167,45 +2748,25 @@
         <v>6.7599999999999993E-2</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="L29" t="s">
-        <v>124</v>
-      </c>
-      <c r="M29" s="1">
-        <v>0.31913828999068994</v>
-      </c>
-      <c r="N29">
-        <f>-2.84/10000</f>
-        <v>-2.8399999999999996E-4</v>
-      </c>
-      <c r="O29">
-        <f>0.18/10000</f>
-        <v>1.8E-5</v>
-      </c>
-      <c r="P29">
-        <f>5.7/100000</f>
-        <v>5.7000000000000003E-5</v>
-      </c>
-      <c r="Q29">
-        <f>4.3/10000000</f>
-        <v>4.2999999999999996E-7</v>
-      </c>
-      <c r="R29" s="45" t="s">
-        <v>148</v>
-      </c>
-      <c r="S29">
-        <v>1.9E-3</v>
-      </c>
-      <c r="U29" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="M29" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="O29" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="V29" s="14" t="s">
+      <c r="P29" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="W29" s="17"/>
-    </row>
-    <row r="30" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q29" s="17" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="12"/>
       <c r="C30" s="1">
@@ -3234,46 +2795,26 @@
         <v>3.2599999999999999E-3</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L30" s="55" t="s">
-        <v>125</v>
-      </c>
-      <c r="M30" s="1">
-        <v>-8.9071075304571687E-2</v>
-      </c>
-      <c r="N30">
-        <f>3.75/10000</f>
-        <v>3.7500000000000001E-4</v>
-      </c>
-      <c r="O30">
-        <f>0.04/10000</f>
-        <v>3.9999999999999998E-6</v>
-      </c>
-      <c r="P30">
-        <f>4.7/100000</f>
-        <v>4.7000000000000004E-5</v>
-      </c>
-      <c r="Q30">
-        <f>1.5/10000000</f>
-        <v>1.4999999999999999E-7</v>
-      </c>
-      <c r="R30" s="45" t="s">
-        <v>149</v>
-      </c>
-      <c r="S30">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="T30" s="1"/>
-      <c r="U30" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="M30" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="N30" s="1"/>
+      <c r="O30" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="V30" s="5" t="s">
+      <c r="P30" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="W30" s="17"/>
-    </row>
-    <row r="31" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q30" s="17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="24"/>
       <c r="C31" s="25">
@@ -3302,46 +2843,26 @@
         <v>1.08</v>
       </c>
       <c r="K31" s="25" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="L31" s="56" t="s">
-        <v>126</v>
-      </c>
-      <c r="M31" s="1">
-        <v>-9.5164725912389475E-2</v>
-      </c>
-      <c r="N31" s="35">
-        <f>3.62/10000</f>
-        <v>3.6200000000000002E-4</v>
-      </c>
-      <c r="O31" s="35">
-        <f>0.03/10000</f>
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="P31" s="35">
-        <f>3.5/100000</f>
-        <v>3.4999999999999997E-5</v>
-      </c>
-      <c r="Q31" s="35">
-        <f>1.5/10000000</f>
-        <v>1.4999999999999999E-7</v>
-      </c>
-      <c r="R31" s="46" t="s">
-        <v>150</v>
-      </c>
-      <c r="S31" s="35">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="T31" s="35"/>
-      <c r="U31" s="26" t="s">
+        <v>120</v>
+      </c>
+      <c r="M31" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="N31" s="35"/>
+      <c r="O31" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="V31" s="50" t="s">
+      <c r="P31" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="W31" s="17"/>
-    </row>
-    <row r="32" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q31" s="17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="12">
         <v>14</v>
@@ -3372,43 +2893,25 @@
         <v>9.18</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="L32" s="55" t="s">
-        <v>127</v>
-      </c>
-      <c r="M32" s="1">
-        <v>-9.6809513242537004E-2</v>
-      </c>
-      <c r="N32">
-        <v>1.1299999999999999E-3</v>
-      </c>
-      <c r="O32">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="P32">
-        <f>1.121/10000</f>
-        <v>1.121E-4</v>
-      </c>
-      <c r="Q32">
-        <f>4.4/10000000</f>
-        <v>4.4000000000000002E-7</v>
-      </c>
-      <c r="R32" s="45" t="s">
-        <v>151</v>
-      </c>
-      <c r="S32">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="U32" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="M32" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="O32" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="V32" s="14" t="s">
+      <c r="P32" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="W32" s="17"/>
-    </row>
-    <row r="33" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q32" s="17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="12"/>
       <c r="C33" s="1">
@@ -3437,43 +2940,25 @@
         <v>15.8</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L33" s="55" t="s">
-        <v>128</v>
-      </c>
-      <c r="M33" s="1">
-        <v>-0.4592253227166484</v>
-      </c>
-      <c r="N33">
-        <v>3.9300000000000003E-3</v>
-      </c>
-      <c r="O33">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="P33">
-        <f>9.3/100000</f>
-        <v>9.3000000000000011E-5</v>
-      </c>
-      <c r="Q33">
-        <f>9/10000000</f>
-        <v>8.9999999999999996E-7</v>
-      </c>
-      <c r="R33" s="45" t="s">
-        <v>152</v>
-      </c>
-      <c r="S33">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="U33" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="M33" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="O33" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="V33" s="5" t="s">
+      <c r="P33" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="W33" s="17"/>
-    </row>
-    <row r="34" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="Q33" s="17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="12"/>
       <c r="C34" s="1">
@@ -3502,45 +2987,25 @@
         <v>12.1</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="L34" s="55" t="s">
-        <v>129</v>
-      </c>
-      <c r="M34" s="1">
-        <v>-4.7584051699129312E-2</v>
-      </c>
-      <c r="N34">
-        <f>8.82/10000</f>
-        <v>8.8200000000000008E-4</v>
-      </c>
-      <c r="O34">
-        <f>0.03/10000</f>
-        <v>3.0000000000000001E-6</v>
-      </c>
-      <c r="P34">
-        <f>6.7/100000</f>
-        <v>6.7000000000000002E-5</v>
-      </c>
-      <c r="Q34">
-        <f>8/100000000</f>
-        <v>8.0000000000000002E-8</v>
-      </c>
-      <c r="R34" s="45" t="s">
-        <v>153</v>
-      </c>
-      <c r="S34">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="U34" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="M34" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="O34" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="V34" s="5" t="s">
+      <c r="P34" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="W34" s="17"/>
-    </row>
-    <row r="35" spans="1:23" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q34" s="17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="19"/>
       <c r="B35" s="20"/>
       <c r="C35" s="6">
@@ -3569,44 +3034,26 @@
         <v>15.7</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L35" s="57" t="s">
-        <v>130</v>
-      </c>
-      <c r="M35" s="1">
-        <v>-0.68631169220488575</v>
-      </c>
-      <c r="N35" s="21">
-        <v>5.1599999999999997E-3</v>
-      </c>
-      <c r="O35" s="21">
-        <v>2.0000000000000002E-5</v>
-      </c>
-      <c r="P35" s="21">
-        <f>9.33/100000</f>
-        <v>9.3300000000000005E-5</v>
-      </c>
-      <c r="Q35" s="21">
-        <f>1.1/1000000</f>
-        <v>1.1000000000000001E-6</v>
-      </c>
-      <c r="R35" s="45" t="s">
-        <v>154</v>
-      </c>
-      <c r="S35">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="T35" s="21"/>
-      <c r="U35" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="M35" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="N35" s="21"/>
+      <c r="O35" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="V35" s="22" t="s">
+      <c r="P35" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="W35" s="17"/>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="Q35" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="J39" s="52">
         <v>1000000</v>
       </c>

</xml_diff>